<commit_message>
Botones de navegacion en RFQ
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="615" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="465" yWindow="615" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="153">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -461,6 +461,24 @@
   </si>
   <si>
     <t>PO DATE</t>
+  </si>
+  <si>
+    <t>TABLE: CONTRACT</t>
+  </si>
+  <si>
+    <t>CONTRACT</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>OC CLIENTE</t>
+  </si>
+  <si>
+    <t>FECHA DEL CONTRATO</t>
+  </si>
+  <si>
+    <t>DIRECCION DEL ARCHIVO</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG65"/>
+  <dimension ref="A1:AO65"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1213,13 +1231,13 @@
     <col min="26" max="26" width="4.5703125" customWidth="1"/>
     <col min="27" max="27" width="14.42578125" customWidth="1"/>
     <col min="28" max="28" width="12.140625" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.28515625" customWidth="1"/>
     <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:41">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1247,7 +1265,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:41">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1274,8 +1292,12 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:33">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+    </row>
+    <row r="3" spans="1:41">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>19</v>
@@ -1312,14 +1334,20 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="2"/>
+      <c r="AI3" t="s">
         <v>142</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AM3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:41">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -1385,17 +1413,27 @@
       <c r="AC4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AD4" s="2"/>
+      <c r="AI4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AK4" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:33">
+      <c r="AM4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -1448,8 +1486,8 @@
       </c>
       <c r="Y5" s="8"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="1" t="s">
-        <v>143</v>
+      <c r="AA5" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>20</v>
@@ -1457,15 +1495,25 @@
       <c r="AC5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AD5" s="2"/>
+      <c r="AI5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AF5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG5" s="1"/>
-    </row>
-    <row r="6" spans="1:33">
+      <c r="AN5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO5" s="1"/>
+    </row>
+    <row r="6" spans="1:41">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -1512,22 +1560,32 @@
       </c>
       <c r="Y6" s="6"/>
       <c r="Z6" s="2"/>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD6" s="2"/>
+      <c r="AI6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AE6" s="1" t="s">
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AM6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AF6" s="6" t="s">
+      <c r="AN6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AO6" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:41">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -1576,20 +1634,28 @@
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="2"/>
+      <c r="AI7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AE7" s="13" t="s">
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AM7" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AN7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AG7" s="1"/>
-    </row>
-    <row r="8" spans="1:33">
+      <c r="AO7" s="1"/>
+    </row>
+    <row r="8" spans="1:41">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -1640,8 +1706,16 @@
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:33">
+      <c r="AA8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="2"/>
+    </row>
+    <row r="9" spans="1:41">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -1686,8 +1760,18 @@
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:33">
+      <c r="AA9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB9" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD9" s="2"/>
+    </row>
+    <row r="10" spans="1:41">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
         <v>8</v>
@@ -1732,8 +1816,18 @@
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:33">
+      <c r="AA10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC10" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD10" s="2"/>
+    </row>
+    <row r="11" spans="1:41">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
@@ -1778,8 +1872,12 @@
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="2"/>
-    </row>
-    <row r="12" spans="1:33">
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="2"/>
+    </row>
+    <row r="12" spans="1:41">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
@@ -1820,8 +1918,12 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
-    </row>
-    <row r="13" spans="1:33">
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+    </row>
+    <row r="13" spans="1:41">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -1864,8 +1966,12 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
-    </row>
-    <row r="14" spans="1:33">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+    </row>
+    <row r="14" spans="1:41">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -1908,8 +2014,12 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
-    </row>
-    <row r="15" spans="1:33">
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+    </row>
+    <row r="15" spans="1:41">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -1948,8 +2058,12 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
-    </row>
-    <row r="16" spans="1:33">
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+    </row>
+    <row r="16" spans="1:41">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -1988,8 +2102,12 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
-    </row>
-    <row r="17" spans="1:26">
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -2026,8 +2144,12 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2058,8 +2180,12 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2090,8 +2216,12 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2122,8 +2252,12 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2156,8 +2290,12 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
-    </row>
-    <row r="22" spans="1:26">
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2190,8 +2328,12 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2224,8 +2366,12 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2258,8 +2404,12 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
-    </row>
-    <row r="25" spans="1:26">
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2286,8 +2436,12 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
-    </row>
-    <row r="26" spans="1:26">
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+    </row>
+    <row r="26" spans="1:30">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2314,8 +2468,12 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2342,8 +2500,12 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
-    </row>
-    <row r="28" spans="1:26">
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+    </row>
+    <row r="28" spans="1:30">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2370,8 +2532,12 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
-    </row>
-    <row r="29" spans="1:26">
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+    </row>
+    <row r="29" spans="1:30">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2398,8 +2564,12 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26">
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+    </row>
+    <row r="30" spans="1:30">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2426,8 +2596,12 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="1:26">
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+    </row>
+    <row r="31" spans="1:30">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2454,8 +2628,12 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26">
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+    </row>
+    <row r="32" spans="1:30">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2482,8 +2660,12 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
-    </row>
-    <row r="33" spans="1:25">
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+    </row>
+    <row r="33" spans="1:30">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2506,8 +2688,13 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+    </row>
+    <row r="34" spans="1:30">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
         <v>78</v>
@@ -2544,7 +2731,7 @@
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:30">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>0</v>
@@ -2601,7 +2788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:30">
       <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
         <v>87</v>
@@ -2658,7 +2845,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:30">
       <c r="A37" s="2"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
@@ -2713,7 +2900,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:30">
       <c r="A38" s="2"/>
       <c r="B38" s="6" t="s">
         <v>4</v>
@@ -2766,7 +2953,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:30">
       <c r="A39" s="2"/>
       <c r="B39" s="6" t="s">
         <v>5</v>
@@ -2819,7 +3006,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:30">
       <c r="A40" s="2"/>
       <c r="B40" s="6" t="s">
         <v>77</v>
@@ -2872,7 +3059,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:30">
       <c r="A41" s="2"/>
       <c r="B41" s="6" t="s">
         <v>62</v>
@@ -2929,7 +3116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:30">
       <c r="A42" s="2"/>
       <c r="B42" s="6" t="s">
         <v>63</v>
@@ -2978,7 +3165,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:30">
       <c r="A43" s="2"/>
       <c r="B43" s="6" t="s">
         <v>64</v>
@@ -3021,7 +3208,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:30">
       <c r="A44" s="2"/>
       <c r="B44" s="6" t="s">
         <v>65</v>
@@ -3064,7 +3251,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:30">
       <c r="A45" s="2"/>
       <c r="B45" s="6" t="s">
         <v>67</v>
@@ -3105,7 +3292,7 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:30">
       <c r="A46" s="2"/>
       <c r="B46" s="6" t="s">
         <v>74</v>
@@ -3146,7 +3333,7 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:30">
       <c r="A47" s="2"/>
       <c r="B47" s="6" t="s">
         <v>68</v>
@@ -3185,7 +3372,7 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:30">
       <c r="A48" s="2"/>
       <c r="B48" s="12" t="s">
         <v>75</v>
@@ -3593,7 +3780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modificacion y actualizacion de modelo y db
Se actualiza las tablas de CONTRACT, PURCHASE ORDERS, TECH INFO EXTERNAL
SERVER y los  modelos que resultaron afectados.

Se crea la tabla FIELD OPERATIONS TECHS
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagarciar\Source\Repos\axis\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="465" yWindow="615" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -13,17 +18,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FIELD VALUES'!$C$60:$E$233</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="449">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1361,16 +1362,25 @@
   </si>
   <si>
     <t>OPEN / CLOSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date auto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es necesario definir los perfiles y los niveles de acceso que tendra </t>
+  </si>
+  <si>
+    <t>cada uno.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,9 +1671,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1682,10 +1692,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1703,7 +1713,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1742,7 +1753,7 @@
         <xdr:cNvPr id="3" name="Elbow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1797,7 +1808,7 @@
         <xdr:cNvPr id="5" name="Elbow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,7 +1863,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1905,7 +1916,7 @@
         <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1958,7 +1969,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2011,7 +2022,7 @@
         <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,7 +2075,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2101,10 +2112,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
@@ -2117,7 +2128,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2125,8 +2136,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20381119" y="1081088"/>
-          <a:ext cx="904875" cy="154781"/>
+          <a:off x="17264062" y="952500"/>
+          <a:ext cx="4105276" cy="283369"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2170,7 +2181,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2223,7 +2234,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2304,7 +2315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2336,9 +2347,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2370,6 +2399,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2545,14 +2592,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -2595,7 +2642,7 @@
     <col min="40" max="40" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2637,7 +2684,7 @@
       <c r="AO1" s="2"/>
       <c r="AP1" s="2"/>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2681,7 +2728,7 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>19</v>
@@ -2741,7 +2788,7 @@
       <c r="AO3" s="30"/>
       <c r="AP3" s="30"/>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -2833,7 +2880,7 @@
       <c r="AO4" s="29"/>
       <c r="AP4" s="29"/>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -2917,7 +2964,7 @@
       <c r="AO5" s="7"/>
       <c r="AP5" s="30"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -2985,19 +3032,19 @@
       </c>
       <c r="AJ6" s="30"/>
       <c r="AK6" s="30"/>
-      <c r="AL6" s="31" t="s">
+      <c r="AL6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="AM6" s="31" t="s">
+      <c r="AM6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="31" t="s">
+      <c r="AN6" s="11" t="s">
         <v>425</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -3067,19 +3114,19 @@
       </c>
       <c r="AJ7" s="30"/>
       <c r="AK7" s="30"/>
-      <c r="AL7" s="31" t="s">
+      <c r="AL7" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="AM7" s="31" t="s">
+      <c r="AM7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AN7" s="31" t="s">
+      <c r="AN7" s="11" t="s">
         <v>442</v>
       </c>
       <c r="AO7" s="30"/>
       <c r="AP7" s="30"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -3153,19 +3200,19 @@
       </c>
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
-      <c r="AL8" s="31" t="s">
+      <c r="AL8" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="AM8" s="31" t="s">
+      <c r="AM8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AN8" s="35" t="s">
+      <c r="AN8" s="36" t="s">
         <v>428</v>
       </c>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -3211,13 +3258,13 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="2"/>
-      <c r="AB9" s="31" t="s">
+      <c r="AB9" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="AC9" s="31" t="s">
+      <c r="AC9" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="AD9" s="31" t="s">
+      <c r="AD9" s="11" t="s">
         <v>414</v>
       </c>
       <c r="AE9" s="2"/>
@@ -3233,19 +3280,19 @@
       </c>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
-      <c r="AL9" s="31" t="s">
+      <c r="AL9" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="AM9" s="31" t="s">
+      <c r="AM9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AN9" s="31" t="s">
+      <c r="AN9" s="11" t="s">
         <v>443</v>
       </c>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
         <v>8</v>
@@ -3291,41 +3338,41 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" s="31" t="s">
+      <c r="AB10" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="AC10" s="31" t="s">
+      <c r="AC10" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="AD10" s="31" t="s">
+      <c r="AD10" s="11" t="s">
         <v>411</v>
       </c>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="31" t="s">
-        <v>424</v>
-      </c>
-      <c r="AH10" s="31" t="s">
-        <v>440</v>
-      </c>
-      <c r="AI10" s="31" t="s">
-        <v>441</v>
+      <c r="AG10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>446</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
-      <c r="AL10" s="31" t="s">
+      <c r="AL10" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="AM10" s="31" t="s">
+      <c r="AM10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AN10" s="31" t="s">
+      <c r="AN10" s="11" t="s">
         <v>434</v>
       </c>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
@@ -3382,30 +3429,30 @@
       </c>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
-      <c r="AG11" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI11" s="31" t="s">
-        <v>444</v>
+      <c r="AG11" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="AH11" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="AI11" s="11" t="s">
+        <v>441</v>
       </c>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
-      <c r="AL11" s="31" t="s">
+      <c r="AL11" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="AM11" s="31" t="s">
+      <c r="AM11" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="AN11" s="31" t="s">
+      <c r="AN11" s="11" t="s">
         <v>437</v>
       </c>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
@@ -3447,35 +3494,41 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="6" t="s">
+      <c r="AB12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AC12" s="6" t="s">
+      <c r="AC12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AD12" s="11" t="s">
         <v>410</v>
       </c>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
-      <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
-      <c r="AI12" s="7"/>
+      <c r="AG12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI12" s="11" t="s">
+        <v>444</v>
+      </c>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
-      <c r="AL12" s="31" t="s">
+      <c r="AL12" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="AM12" s="31" t="s">
+      <c r="AM12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AN12" s="31" t="s">
+      <c r="AN12" s="11" t="s">
         <v>439</v>
       </c>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -3519,13 +3572,13 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="8" t="s">
+      <c r="AB13" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" s="6" t="s">
+      <c r="AC13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AD13" s="8" t="s">
+      <c r="AD13" s="35" t="s">
         <v>445</v>
       </c>
       <c r="AE13" s="2"/>
@@ -3541,7 +3594,7 @@
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -3601,7 +3654,7 @@
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -3657,7 +3710,7 @@
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -3707,13 +3760,15 @@
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
-      <c r="AL16" s="2"/>
+      <c r="AL16" s="2" t="s">
+        <v>447</v>
+      </c>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="2"/>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -3761,13 +3816,15 @@
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
+      <c r="AL17" s="2" t="s">
+        <v>448</v>
+      </c>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3815,7 +3872,7 @@
       <c r="AO18" s="2"/>
       <c r="AP18" s="2"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3863,7 +3920,7 @@
       <c r="AO19" s="2"/>
       <c r="AP19" s="2"/>
     </row>
-    <row r="20" spans="1:42">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3911,7 +3968,7 @@
       <c r="AO20" s="2"/>
       <c r="AP20" s="2"/>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3961,7 +4018,7 @@
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4011,7 +4068,7 @@
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4061,7 +4118,7 @@
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4111,7 +4168,7 @@
       <c r="AO24" s="2"/>
       <c r="AP24" s="2"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4155,7 +4212,7 @@
       <c r="AO25" s="2"/>
       <c r="AP25" s="2"/>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4199,7 +4256,7 @@
       <c r="AO26" s="2"/>
       <c r="AP26" s="2"/>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4243,7 +4300,7 @@
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4287,7 +4344,7 @@
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4331,7 +4388,7 @@
       <c r="AO29" s="2"/>
       <c r="AP29" s="2"/>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4375,7 +4432,7 @@
       <c r="AO30" s="2"/>
       <c r="AP30" s="2"/>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4419,7 +4476,7 @@
       <c r="AO31" s="2"/>
       <c r="AP31" s="2"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4463,7 +4520,7 @@
       <c r="AO32" s="2"/>
       <c r="AP32" s="2"/>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4503,7 +4560,7 @@
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
     </row>
-    <row r="34" spans="1:42">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
         <v>77</v>
@@ -4541,7 +4598,7 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row r="35" spans="1:42">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>0</v>
@@ -4600,7 +4657,7 @@
       <c r="Z35" s="29"/>
       <c r="AC35" s="29"/>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
         <v>82</v>
@@ -4658,7 +4715,7 @@
       </c>
       <c r="Z36" s="30"/>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
@@ -4714,7 +4771,7 @@
       </c>
       <c r="Z37" s="30"/>
     </row>
-    <row r="38" spans="1:42">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="6" t="s">
         <v>4</v>
@@ -4770,7 +4827,7 @@
       </c>
       <c r="Z38" s="30"/>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="6" t="s">
         <v>5</v>
@@ -4826,7 +4883,7 @@
       </c>
       <c r="Z39" s="30"/>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="6" t="s">
         <v>76</v>
@@ -4882,7 +4939,7 @@
       </c>
       <c r="Z40" s="30"/>
     </row>
-    <row r="41" spans="1:42">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="6" t="s">
         <v>134</v>
@@ -4942,7 +4999,7 @@
       </c>
       <c r="Z41" s="30"/>
     </row>
-    <row r="42" spans="1:42">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="6" t="s">
         <v>135</v>
@@ -4993,7 +5050,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="6" t="s">
         <v>14</v>
@@ -5038,7 +5095,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="6" t="s">
         <v>136</v>
@@ -5083,7 +5140,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:42">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="6" t="s">
         <v>16</v>
@@ -5128,7 +5185,7 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="6" t="s">
         <v>62</v>
@@ -5173,7 +5230,7 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="6" t="s">
         <v>63</v>
@@ -5218,7 +5275,7 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:42">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="6" t="s">
         <v>64</v>
@@ -5263,7 +5320,7 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="6" t="s">
         <v>66</v>
@@ -5306,7 +5363,7 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="6" t="s">
         <v>73</v>
@@ -5349,7 +5406,7 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="6" t="s">
         <v>67</v>
@@ -5383,7 +5440,7 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="6" t="s">
         <v>74</v>
@@ -5420,7 +5477,7 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
@@ -5451,7 +5508,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="6" t="s">
         <v>69</v>
@@ -5484,7 +5541,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="6" t="s">
         <v>70</v>
@@ -5512,7 +5569,7 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="6" t="s">
         <v>71</v>
@@ -5540,7 +5597,7 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="6" t="s">
         <v>72</v>
@@ -5568,7 +5625,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58" s="31" t="s">
         <v>39</v>
       </c>
@@ -5588,7 +5645,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B59" s="31" t="s">
         <v>431</v>
       </c>
@@ -5606,7 +5663,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:22">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M60" s="8" t="s">
         <v>128</v>
       </c>
@@ -5621,24 +5678,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="C2:M290"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -5649,7 +5701,7 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:13">
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
@@ -5665,7 +5717,7 @@
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="4:13">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
         <v>58</v>
       </c>
@@ -5681,7 +5733,7 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="4:13">
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D4" s="12" t="s">
         <v>58</v>
       </c>
@@ -5698,7 +5750,7 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="4:13">
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>58</v>
       </c>
@@ -5715,7 +5767,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="4:13">
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D6" s="12" t="s">
         <v>58</v>
       </c>
@@ -5732,7 +5784,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="4:13">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>58</v>
       </c>
@@ -5749,7 +5801,7 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="4:13">
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>58</v>
       </c>
@@ -5766,7 +5818,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="4:13">
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
@@ -5783,7 +5835,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="4:13">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
@@ -5800,7 +5852,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="4:13">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D11" s="12" t="s">
         <v>58</v>
       </c>
@@ -5817,7 +5869,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="4:13">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D12" s="12" t="s">
         <v>58</v>
       </c>
@@ -5834,7 +5886,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="4:13">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D13" s="12" t="s">
         <v>58</v>
       </c>
@@ -5851,7 +5903,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="4:13">
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D14" s="12" t="s">
         <v>58</v>
       </c>
@@ -5868,7 +5920,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="4:13">
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D15" s="12" t="s">
         <v>58</v>
       </c>
@@ -5885,7 +5937,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="4:13">
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>58</v>
       </c>
@@ -5902,7 +5954,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="4:13">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" s="13" t="s">
         <v>59</v>
       </c>
@@ -5919,7 +5971,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="4:13">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" s="13" t="s">
         <v>59</v>
       </c>
@@ -5936,7 +5988,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="4:13">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D19" s="13" t="s">
         <v>59</v>
       </c>
@@ -5953,7 +6005,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="4:13">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D20" s="13" t="s">
         <v>59</v>
       </c>
@@ -5970,7 +6022,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="4:13">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D21" s="13" t="s">
         <v>59</v>
       </c>
@@ -5987,7 +6039,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="4:13">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" s="13" t="s">
         <v>59</v>
       </c>
@@ -5996,7 +6048,7 @@
         <v>CONSTRUCT: COMMISION</v>
       </c>
     </row>
-    <row r="23" spans="4:13">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D23" s="13" t="s">
         <v>59</v>
       </c>
@@ -6005,7 +6057,7 @@
         <v>CONSTRUCT: OPEN</v>
       </c>
     </row>
-    <row r="26" spans="4:13">
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D26" s="14" t="s">
         <v>149</v>
       </c>
@@ -6013,73 +6065,73 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="4:13">
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="4:13">
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="4:13">
+    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="4:13">
+    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="4:13">
+    <row r="31" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="4:13">
+    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="4:11">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="4:11">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="4:11">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="4:11">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="4:11">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="4:11" ht="15.75" thickBot="1">
+    <row r="42" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>162</v>
       </c>
@@ -6087,7 +6139,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="4:11" ht="24.75" thickBot="1">
+    <row r="43" spans="4:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D43" s="15" t="s">
         <v>49</v>
       </c>
@@ -6101,7 +6153,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="4:11">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="16" t="s">
         <v>167</v>
       </c>
@@ -6113,7 +6165,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="4:11">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="20" t="s">
         <v>168</v>
       </c>
@@ -6125,7 +6177,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="4:11">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="20" t="s">
         <v>165</v>
       </c>
@@ -6135,7 +6187,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="4:11">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="20" t="s">
         <v>165</v>
       </c>
@@ -6145,7 +6197,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="4:11">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="20" t="s">
         <v>171</v>
       </c>
@@ -6157,7 +6209,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="49" spans="3:7">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D49" s="20" t="s">
         <v>172</v>
       </c>
@@ -6169,7 +6221,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="50" spans="3:7">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D50" s="20" t="s">
         <v>173</v>
       </c>
@@ -6179,7 +6231,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="22"/>
     </row>
-    <row r="51" spans="3:7">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D51" s="20" t="s">
         <v>174</v>
       </c>
@@ -6189,7 +6241,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="22"/>
     </row>
-    <row r="52" spans="3:7">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D52" s="20" t="s">
         <v>175</v>
       </c>
@@ -6199,7 +6251,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="3:7">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D53" s="20" t="s">
         <v>176</v>
       </c>
@@ -6209,7 +6261,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="22"/>
     </row>
-    <row r="54" spans="3:7">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D54" s="20" t="s">
         <v>178</v>
       </c>
@@ -6219,7 +6271,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="3:7">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D55" s="20" t="s">
         <v>179</v>
       </c>
@@ -6229,7 +6281,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="3:7">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D56" s="20" t="s">
         <v>180</v>
       </c>
@@ -6239,7 +6291,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="22"/>
     </row>
-    <row r="57" spans="3:7" ht="15.75" thickBot="1">
+    <row r="57" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="23" t="s">
         <v>181</v>
       </c>
@@ -6249,7 +6301,7 @@
       <c r="F57" s="24"/>
       <c r="G57" s="25"/>
     </row>
-    <row r="60" spans="3:7">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>405</v>
       </c>
@@ -6260,7 +6312,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="61" spans="3:7" hidden="1">
+    <row r="61" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" s="28">
         <v>1</v>
       </c>
@@ -6275,7 +6327,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('AAER', 'A1500-77');</v>
       </c>
     </row>
-    <row r="62" spans="3:7" hidden="1">
+    <row r="62" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" s="28">
         <f>+C61+1</f>
         <v>2</v>
@@ -6291,7 +6343,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('AAER', 'A1500-70');</v>
       </c>
     </row>
-    <row r="63" spans="3:7" hidden="1">
+    <row r="63" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" s="28">
         <f t="shared" ref="C63:C126" si="1">+C62+1</f>
         <v>3</v>
@@ -6307,7 +6359,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW3000-116');</v>
       </c>
     </row>
-    <row r="64" spans="3:7" hidden="1">
+    <row r="64" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" s="28">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -6323,7 +6375,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW3000-109');</v>
       </c>
     </row>
-    <row r="65" spans="3:7" hidden="1">
+    <row r="65" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C65" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6339,7 +6391,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW1500-82');</v>
       </c>
     </row>
-    <row r="66" spans="3:7" hidden="1">
+    <row r="66" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C66" s="28">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6355,7 +6407,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW1500-77');</v>
       </c>
     </row>
-    <row r="67" spans="3:7" hidden="1">
+    <row r="67" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C67" s="28">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6371,7 +6423,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeroman', 'Aeroman 14.8');</v>
       </c>
     </row>
-    <row r="68" spans="3:7" hidden="1">
+    <row r="68" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" s="28">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6387,7 +6439,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeronautica', 'Aeronautic 47');</v>
       </c>
     </row>
-    <row r="69" spans="3:7" hidden="1">
+    <row r="69" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C69" s="28">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6403,7 +6455,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeronautica', 'A54-750');</v>
       </c>
     </row>
-    <row r="70" spans="3:7" hidden="1">
+    <row r="70" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C70" s="28">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6419,7 +6471,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Alstom', 'ECO100');</v>
       </c>
     </row>
-    <row r="71" spans="3:7" hidden="1">
+    <row r="71" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" s="28">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -6435,7 +6487,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Alstom', 'ECO86');</v>
       </c>
     </row>
-    <row r="72" spans="3:7" hidden="1">
+    <row r="72" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" s="28">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6451,7 +6503,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Atlantic Orient', 'AOC 15/50');</v>
       </c>
     </row>
-    <row r="73" spans="3:7">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="28">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -6467,7 +6519,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Bergey Windpower', 'XL50');</v>
       </c>
     </row>
-    <row r="74" spans="3:7" hidden="1">
+    <row r="74" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74" s="28">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -6483,7 +6535,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('CCWE', 'CCWE-3600D/115');</v>
       </c>
     </row>
-    <row r="75" spans="3:7" hidden="1">
+    <row r="75" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C75" s="28">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -6499,7 +6551,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-96');</v>
       </c>
     </row>
-    <row r="76" spans="3:7" hidden="1">
+    <row r="76" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="28">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -6515,7 +6567,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-93');</v>
       </c>
     </row>
-    <row r="77" spans="3:7" hidden="1">
+    <row r="77" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C77" s="28">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -6531,7 +6583,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-89');</v>
       </c>
     </row>
-    <row r="78" spans="3:7" hidden="1">
+    <row r="78" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C78" s="28">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -6547,7 +6599,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Daewoo Dewind', 'D8.2');</v>
       </c>
     </row>
-    <row r="79" spans="3:7" hidden="1">
+    <row r="79" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C79" s="28">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -6563,7 +6615,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Daewoo Dewind', 'D9.2');</v>
       </c>
     </row>
-    <row r="80" spans="3:7" hidden="1">
+    <row r="80" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C80" s="28">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -6579,7 +6631,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Danwin', '23 E2');</v>
       </c>
     </row>
-    <row r="81" spans="3:7" hidden="1">
+    <row r="81" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C81" s="28">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -6595,7 +6647,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Danwin', '24/160');</v>
       </c>
     </row>
-    <row r="82" spans="3:7" hidden="1">
+    <row r="82" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C82" s="28">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -6611,7 +6663,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('DES', 'Northwind 100');</v>
       </c>
     </row>
-    <row r="83" spans="3:7" hidden="1">
+    <row r="83" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C83" s="28">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -6627,7 +6679,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Eastern Wind Power', 'Sky Farm 50kW VAWT');</v>
       </c>
     </row>
-    <row r="84" spans="3:7" hidden="1">
+    <row r="84" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" s="28">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -6643,7 +6695,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Elecon', 'T600-48');</v>
       </c>
     </row>
-    <row r="85" spans="3:7" hidden="1">
+    <row r="85" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C85" s="28">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -6659,7 +6711,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Elecon', 'T600-48DS');</v>
       </c>
     </row>
-    <row r="86" spans="3:7" hidden="1">
+    <row r="86" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C86" s="28">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -6675,7 +6727,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Endurance', 'E3120 50kW');</v>
       </c>
     </row>
-    <row r="87" spans="3:7" hidden="1">
+    <row r="87" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C87" s="28">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -6691,7 +6743,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Enertech', 'E48');</v>
       </c>
     </row>
-    <row r="88" spans="3:7" hidden="1">
+    <row r="88" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C88" s="28">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -6707,7 +6759,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Enertech', 'Enertech 44/40');</v>
       </c>
     </row>
-    <row r="89" spans="3:7" hidden="1">
+    <row r="89" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C89" s="28">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -6723,7 +6775,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW54-900');</v>
       </c>
     </row>
-    <row r="90" spans="3:7" hidden="1">
+    <row r="90" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C90" s="28">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -6739,7 +6791,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW52-750');</v>
       </c>
     </row>
-    <row r="91" spans="3:7" hidden="1">
+    <row r="91" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C91" s="28">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -6755,7 +6807,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW52-900');</v>
       </c>
     </row>
-    <row r="92" spans="3:7" hidden="1">
+    <row r="92" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C92" s="28">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -6771,7 +6823,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL1500');</v>
       </c>
     </row>
-    <row r="93" spans="3:7" hidden="1">
+    <row r="93" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C93" s="28">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -6787,7 +6839,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL100');</v>
       </c>
     </row>
-    <row r="94" spans="3:7" hidden="1">
+    <row r="94" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C94" s="28">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -6803,7 +6855,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL250');</v>
       </c>
     </row>
-    <row r="95" spans="3:7" hidden="1">
+    <row r="95" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C95" s="28">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6819,7 +6871,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL2500/90');</v>
       </c>
     </row>
-    <row r="96" spans="3:7" hidden="1">
+    <row r="96" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C96" s="28">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -6835,7 +6887,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G97-2.0');</v>
       </c>
     </row>
-    <row r="97" spans="3:7" hidden="1">
+    <row r="97" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C97" s="28">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -6851,7 +6903,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G90-2.0');</v>
       </c>
     </row>
-    <row r="98" spans="3:7" hidden="1">
+    <row r="98" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C98" s="28">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -6867,7 +6919,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G52-850');</v>
       </c>
     </row>
-    <row r="99" spans="3:7" hidden="1">
+    <row r="99" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C99" s="28">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -6883,7 +6935,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G87-2.0');</v>
       </c>
     </row>
-    <row r="100" spans="3:7" hidden="1">
+    <row r="100" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C100" s="28">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -6899,7 +6951,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G58-850');</v>
       </c>
     </row>
-    <row r="101" spans="3:7" hidden="1">
+    <row r="101" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C101" s="28">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -6915,7 +6967,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G114-2.0');</v>
       </c>
     </row>
-    <row r="102" spans="3:7" hidden="1">
+    <row r="102" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C102" s="28">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -6931,7 +6983,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G83-2.0');</v>
       </c>
     </row>
-    <row r="103" spans="3:7" hidden="1">
+    <row r="103" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C103" s="28">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6947,7 +6999,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G80-2.0');</v>
       </c>
     </row>
-    <row r="104" spans="3:7">
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C104" s="28">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -6963,7 +7015,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.6 XLE');</v>
       </c>
     </row>
-    <row r="105" spans="3:7">
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C105" s="28">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -6979,7 +7031,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SLE');</v>
       </c>
     </row>
-    <row r="106" spans="3:7">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C106" s="28">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -6995,7 +7047,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.85-82.5');</v>
       </c>
     </row>
-    <row r="107" spans="3:7">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" s="28">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -7011,7 +7063,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.6-100');</v>
       </c>
     </row>
-    <row r="108" spans="3:7">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="28">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -7027,7 +7079,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 XLE');</v>
       </c>
     </row>
-    <row r="109" spans="3:7">
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="28">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -7043,7 +7095,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.85-87');</v>
       </c>
     </row>
-    <row r="110" spans="3:7">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C110" s="28">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -7059,7 +7111,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-50');</v>
       </c>
     </row>
-    <row r="111" spans="3:7">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C111" s="28">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -7075,7 +7127,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.68-82.5');</v>
       </c>
     </row>
-    <row r="112" spans="3:7">
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C112" s="28">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -7091,7 +7143,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 S');</v>
       </c>
     </row>
-    <row r="113" spans="3:7">
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C113" s="28">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -7107,7 +7159,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.85-103');</v>
       </c>
     </row>
-    <row r="114" spans="3:7">
+    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C114" s="28">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -7123,7 +7175,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.5-120');</v>
       </c>
     </row>
-    <row r="115" spans="3:7">
+    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C115" s="28">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -7139,7 +7191,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.7-100');</v>
       </c>
     </row>
-    <row r="116" spans="3:7">
+    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" s="28">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -7155,7 +7207,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.7-103');</v>
       </c>
     </row>
-    <row r="117" spans="3:7">
+    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" s="28">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -7171,7 +7223,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-40');</v>
       </c>
     </row>
-    <row r="118" spans="3:7">
+    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C118" s="28">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -7187,7 +7239,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5SL');</v>
       </c>
     </row>
-    <row r="119" spans="3:7">
+    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C119" s="28">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -7203,7 +7255,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', '1.5s (Enron)');</v>
       </c>
     </row>
-    <row r="120" spans="3:7">
+    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C120" s="28">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -7219,7 +7271,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SE');</v>
       </c>
     </row>
-    <row r="121" spans="3:7">
+    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C121" s="28">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -7235,7 +7287,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.5-100');</v>
       </c>
     </row>
-    <row r="122" spans="3:7">
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C122" s="28">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -7251,7 +7303,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SL');</v>
       </c>
     </row>
-    <row r="123" spans="3:7">
+    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C123" s="28">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -7267,7 +7319,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-48');</v>
       </c>
     </row>
-    <row r="124" spans="3:7" hidden="1">
+    <row r="124" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C124" s="28">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -7283,7 +7335,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW82');</v>
       </c>
     </row>
-    <row r="125" spans="3:7" hidden="1">
+    <row r="125" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C125" s="28">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -7299,7 +7351,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW87');</v>
       </c>
     </row>
-    <row r="126" spans="3:7" hidden="1">
+    <row r="126" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C126" s="28">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -7315,7 +7367,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW100-2.5');</v>
       </c>
     </row>
-    <row r="127" spans="3:7" hidden="1">
+    <row r="127" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C127" s="28">
         <f t="shared" ref="C127:C190" si="3">+C126+1</f>
         <v>67</v>
@@ -7331,7 +7383,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW77');</v>
       </c>
     </row>
-    <row r="128" spans="3:7" hidden="1">
+    <row r="128" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C128" s="28">
         <f t="shared" si="3"/>
         <v>68</v>
@@ -7347,7 +7399,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('HHI', 'HQ2000');</v>
       </c>
     </row>
-    <row r="129" spans="3:7" hidden="1">
+    <row r="129" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C129" s="28">
         <f t="shared" si="3"/>
         <v>69</v>
@@ -7363,7 +7415,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('HHI', 'HQ1650');</v>
       </c>
     </row>
-    <row r="130" spans="3:7" hidden="1">
+    <row r="130" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C130" s="28">
         <f t="shared" si="3"/>
         <v>70</v>
@@ -7379,7 +7431,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Jonica Impianti', 'JIMP25');</v>
       </c>
     </row>
-    <row r="131" spans="3:7" hidden="1">
+    <row r="131" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C131" s="28">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -7395,7 +7447,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Kenersys', 'K100');</v>
       </c>
     </row>
-    <row r="132" spans="3:7" hidden="1">
+    <row r="132" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C132" s="28">
         <f t="shared" si="3"/>
         <v>72</v>
@@ -7411,7 +7463,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Kenetech', '56-100');</v>
       </c>
     </row>
-    <row r="133" spans="3:7" hidden="1">
+    <row r="133" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C133" s="28">
         <f t="shared" si="3"/>
         <v>73</v>
@@ -7427,7 +7479,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Leitwind', 'LTW77-1.5');</v>
       </c>
     </row>
-    <row r="134" spans="3:7" hidden="1">
+    <row r="134" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C134" s="28">
         <f t="shared" si="3"/>
         <v>74</v>
@@ -7443,7 +7495,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT62/1.0');</v>
       </c>
     </row>
-    <row r="135" spans="3:7" hidden="1">
+    <row r="135" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C135" s="28">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -7459,7 +7511,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-1000');</v>
       </c>
     </row>
-    <row r="136" spans="3:7" hidden="1">
+    <row r="136" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C136" s="28">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -7475,7 +7527,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT92/2.4');</v>
       </c>
     </row>
-    <row r="137" spans="3:7" hidden="1">
+    <row r="137" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C137" s="28">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -7491,7 +7543,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-600');</v>
       </c>
     </row>
-    <row r="138" spans="3:7" hidden="1">
+    <row r="138" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C138" s="28">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -7507,7 +7559,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT95/2.4');</v>
       </c>
     </row>
-    <row r="139" spans="3:7" hidden="1">
+    <row r="139" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C139" s="28">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -7523,7 +7575,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-250');</v>
       </c>
     </row>
-    <row r="140" spans="3:7" hidden="1">
+    <row r="140" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C140" s="28">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -7539,7 +7591,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT102/2.4');</v>
       </c>
     </row>
-    <row r="141" spans="3:7" hidden="1">
+    <row r="141" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C141" s="28">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -7555,7 +7607,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT100/2.4');</v>
       </c>
     </row>
-    <row r="142" spans="3:7" hidden="1">
+    <row r="142" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C142" s="28">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -7571,7 +7623,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N54/1000');</v>
       </c>
     </row>
-    <row r="143" spans="3:7" hidden="1">
+    <row r="143" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C143" s="28">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -7587,7 +7639,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N43/600');</v>
       </c>
     </row>
-    <row r="144" spans="3:7" hidden="1">
+    <row r="144" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C144" s="28">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -7603,7 +7655,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2300');</v>
       </c>
     </row>
-    <row r="145" spans="3:7" hidden="1">
+    <row r="145" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C145" s="28">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -7619,7 +7671,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N60/1300');</v>
       </c>
     </row>
-    <row r="146" spans="3:7" hidden="1">
+    <row r="146" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C146" s="28">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -7635,7 +7687,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N100/2500');</v>
       </c>
     </row>
-    <row r="147" spans="3:7" hidden="1">
+    <row r="147" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C147" s="28">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -7651,7 +7703,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2500 LS');</v>
       </c>
     </row>
-    <row r="148" spans="3:7" hidden="1">
+    <row r="148" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C148" s="28">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -7667,7 +7719,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2500 HS');</v>
       </c>
     </row>
-    <row r="149" spans="3:7" hidden="1">
+    <row r="149" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C149" s="28">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -7683,7 +7735,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N117/2400');</v>
       </c>
     </row>
-    <row r="150" spans="3:7" hidden="1">
+    <row r="150" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C150" s="28">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -7699,7 +7751,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordic', 'N1000');</v>
       </c>
     </row>
-    <row r="151" spans="3:7" hidden="1">
+    <row r="151" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C151" s="28">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -7715,7 +7767,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Northern Power Systems', 'NPS 100');</v>
       </c>
     </row>
-    <row r="152" spans="3:7" hidden="1">
+    <row r="152" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C152" s="28">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -7731,7 +7783,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Northern Power Systems', 'NPS Prototype');</v>
       </c>
     </row>
-    <row r="153" spans="3:7" hidden="1">
+    <row r="153" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C153">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -7747,7 +7799,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Pioneer', 'P-1650');</v>
       </c>
     </row>
-    <row r="154" spans="3:7" hidden="1">
+    <row r="154" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C154">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -7763,7 +7815,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('PowerWind', 'PowerWind 56');</v>
       </c>
     </row>
-    <row r="155" spans="3:7" hidden="1">
+    <row r="155" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C155">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -7779,7 +7831,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Renewegy', 'VP-20');</v>
       </c>
     </row>
-    <row r="156" spans="3:7" hidden="1">
+    <row r="156" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C156">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -7795,7 +7847,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('RRB Energy', 'PS-600');</v>
       </c>
     </row>
-    <row r="157" spans="3:7" hidden="1">
+    <row r="157" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C157">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -7811,7 +7863,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE100/2.0');</v>
       </c>
     </row>
-    <row r="158" spans="3:7" hidden="1">
+    <row r="158" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C158">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -7827,7 +7879,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE93/2.0');</v>
       </c>
     </row>
-    <row r="159" spans="3:7" hidden="1">
+    <row r="159" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C159">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -7843,7 +7895,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE8720IIIE');</v>
       </c>
     </row>
-    <row r="160" spans="3:7" hidden="1">
+    <row r="160" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C160">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -7859,7 +7911,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Senvion', 'MM92');</v>
       </c>
     </row>
-    <row r="161" spans="3:7" hidden="1">
+    <row r="161" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C161">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -7875,7 +7927,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('SHI', 'SHI2.5-100');</v>
       </c>
     </row>
-    <row r="162" spans="3:7" hidden="1">
+    <row r="162" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C162">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -7891,7 +7943,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B19/120');</v>
       </c>
     </row>
-    <row r="163" spans="3:7" hidden="1">
+    <row r="163" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C163">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -7907,7 +7959,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-101');</v>
       </c>
     </row>
-    <row r="164" spans="3:7" hidden="1">
+    <row r="164" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C164">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -7923,7 +7975,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B37/450');</v>
       </c>
     </row>
-    <row r="165" spans="3:7" hidden="1">
+    <row r="165" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C165">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -7939,7 +7991,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-93');</v>
       </c>
     </row>
-    <row r="166" spans="3:7" hidden="1">
+    <row r="166" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C166">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -7955,7 +8007,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT3.0-101');</v>
       </c>
     </row>
-    <row r="167" spans="3:7" hidden="1">
+    <row r="167" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C167">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -7971,7 +8023,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-108');</v>
       </c>
     </row>
-    <row r="168" spans="3:7" hidden="1">
+    <row r="168" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C168">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -7987,7 +8039,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B62/1300');</v>
       </c>
     </row>
-    <row r="169" spans="3:7" hidden="1">
+    <row r="169" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C169">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -8003,7 +8055,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT-2.3');</v>
       </c>
     </row>
-    <row r="170" spans="3:7" hidden="1">
+    <row r="170" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C170">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -8019,7 +8071,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B15/65');</v>
       </c>
     </row>
-    <row r="171" spans="3:7" hidden="1">
+    <row r="171" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C171">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -8035,7 +8087,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT3.0-113');</v>
       </c>
     </row>
-    <row r="172" spans="3:7" hidden="1">
+    <row r="172" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C172">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -8051,7 +8103,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B23/150');</v>
       </c>
     </row>
-    <row r="173" spans="3:7" hidden="1">
+    <row r="173" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C173">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -8067,7 +8119,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sinovel', 'SL 3000/90');</v>
       </c>
     </row>
-    <row r="174" spans="3:7" hidden="1">
+    <row r="174" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C174">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -8083,7 +8135,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sinovel', 'SL 1500/82');</v>
       </c>
     </row>
-    <row r="175" spans="3:7" hidden="1">
+    <row r="175" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C175">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -8099,7 +8151,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siva', '250/50');</v>
       </c>
     </row>
-    <row r="176" spans="3:7" hidden="1">
+    <row r="176" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C176">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -8115,7 +8167,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S88-2.1');</v>
       </c>
     </row>
-    <row r="177" spans="3:7" hidden="1">
+    <row r="177" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C177">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -8131,7 +8183,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S64-1.25');</v>
       </c>
     </row>
-    <row r="178" spans="3:7" hidden="1">
+    <row r="178" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C178">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -8147,7 +8199,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S95-2.1');</v>
       </c>
     </row>
-    <row r="179" spans="3:7" hidden="1">
+    <row r="179" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C179">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -8163,7 +8215,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S97-2.1');</v>
       </c>
     </row>
-    <row r="180" spans="3:7" hidden="1">
+    <row r="180" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C180">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -8179,7 +8231,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Turbowinds', 'T600-48');</v>
       </c>
     </row>
-    <row r="181" spans="3:7" hidden="1">
+    <row r="181" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C181">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -8195,7 +8247,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Turbowinds', 'T400-34');</v>
       </c>
     </row>
-    <row r="182" spans="3:7" hidden="1">
+    <row r="182" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C182">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -8211,7 +8263,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Unison', 'U54');</v>
       </c>
     </row>
-    <row r="183" spans="3:7" hidden="1">
+    <row r="183" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C183">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -8227,7 +8279,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vanguard', '95T');</v>
       </c>
     </row>
-    <row r="184" spans="3:7" hidden="1">
+    <row r="184" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C184">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -8243,7 +8295,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', 'Vensys 70');</v>
       </c>
     </row>
-    <row r="185" spans="3:7" hidden="1">
+    <row r="185" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C185">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -8259,7 +8311,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', 'Vensys 82');</v>
       </c>
     </row>
-    <row r="186" spans="3:7" hidden="1">
+    <row r="186" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C186">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -8275,7 +8327,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', ' Vensys 77');</v>
       </c>
     </row>
-    <row r="187" spans="3:7" hidden="1">
+    <row r="187" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C187">
         <f t="shared" si="3"/>
         <v>127</v>
@@ -8291,7 +8343,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vergnet', 'MP-R');</v>
       </c>
     </row>
-    <row r="188" spans="3:7" hidden="1">
+    <row r="188" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C188">
         <f t="shared" si="3"/>
         <v>128</v>
@@ -8307,7 +8359,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V27-225');</v>
       </c>
     </row>
-    <row r="189" spans="3:7" hidden="1">
+    <row r="189" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C189">
         <f t="shared" si="3"/>
         <v>129</v>
@@ -8323,7 +8375,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M108/19');</v>
       </c>
     </row>
-    <row r="190" spans="3:7" hidden="1">
+    <row r="190" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C190">
         <f t="shared" si="3"/>
         <v>130</v>
@@ -8339,7 +8391,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM54/950');</v>
       </c>
     </row>
-    <row r="191" spans="3:7" hidden="1">
+    <row r="191" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C191">
         <f t="shared" ref="C191:C233" si="5">+C190+1</f>
         <v>131</v>
@@ -8355,7 +8407,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM52/900');</v>
       </c>
     </row>
-    <row r="192" spans="3:7" hidden="1">
+    <row r="192" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C192">
         <f t="shared" si="5"/>
         <v>132</v>
@@ -8371,7 +8423,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NTK500/37');</v>
       </c>
     </row>
-    <row r="193" spans="3:7" hidden="1">
+    <row r="193" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C193">
         <f t="shared" si="5"/>
         <v>133</v>
@@ -8387,7 +8439,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V42');</v>
       </c>
     </row>
-    <row r="194" spans="3:7" hidden="1">
+    <row r="194" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C194">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -8403,7 +8455,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V47-660');</v>
       </c>
     </row>
-    <row r="195" spans="3:7" hidden="1">
+    <row r="195" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C195">
         <f t="shared" si="5"/>
         <v>135</v>
@@ -8419,7 +8471,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM48/750');</v>
       </c>
     </row>
-    <row r="196" spans="3:7" hidden="1">
+    <row r="196" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C196">
         <f t="shared" si="5"/>
         <v>136</v>
@@ -8435,7 +8487,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V100-1.8');</v>
       </c>
     </row>
-    <row r="197" spans="3:7" hidden="1">
+    <row r="197" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C197">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -8451,7 +8503,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V82-1.65');</v>
       </c>
     </row>
-    <row r="198" spans="3:7" hidden="1">
+    <row r="198" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C198">
         <f t="shared" si="5"/>
         <v>138</v>
@@ -8467,7 +8519,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM82/1650');</v>
       </c>
     </row>
-    <row r="199" spans="3:7" hidden="1">
+    <row r="199" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C199">
         <f t="shared" si="5"/>
         <v>139</v>
@@ -8483,7 +8535,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V44-600');</v>
       </c>
     </row>
-    <row r="200" spans="3:7" hidden="1">
+    <row r="200" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C200">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -8499,7 +8551,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NTK65/17');</v>
       </c>
     </row>
-    <row r="201" spans="3:7" hidden="1">
+    <row r="201" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C201">
         <f t="shared" si="5"/>
         <v>141</v>
@@ -8515,7 +8567,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM44/750');</v>
       </c>
     </row>
-    <row r="202" spans="3:7" hidden="1">
+    <row r="202" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C202">
         <f t="shared" si="5"/>
         <v>142</v>
@@ -8531,7 +8583,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'W250/29');</v>
       </c>
     </row>
-    <row r="203" spans="3:7" hidden="1">
+    <row r="203" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C203">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -8547,7 +8599,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V80-1.8');</v>
       </c>
     </row>
-    <row r="204" spans="3:7" hidden="1">
+    <row r="204" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C204">
         <f t="shared" si="5"/>
         <v>144</v>
@@ -8563,7 +8615,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM950/54');</v>
       </c>
     </row>
-    <row r="205" spans="3:7" hidden="1">
+    <row r="205" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C205">
         <f t="shared" si="5"/>
         <v>145</v>
@@ -8579,7 +8631,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M700/225');</v>
       </c>
     </row>
-    <row r="206" spans="3:7" hidden="1">
+    <row r="206" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C206">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -8595,7 +8647,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM72c/1500');</v>
       </c>
     </row>
-    <row r="207" spans="3:7" hidden="1">
+    <row r="207" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C207">
         <f t="shared" si="5"/>
         <v>147</v>
@@ -8611,7 +8663,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17');</v>
       </c>
     </row>
-    <row r="208" spans="3:7" hidden="1">
+    <row r="208" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C208">
         <f t="shared" si="5"/>
         <v>148</v>
@@ -8627,7 +8679,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V39-500');</v>
       </c>
     </row>
-    <row r="209" spans="3:7" hidden="1">
+    <row r="209" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C209">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -8643,7 +8695,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V27');</v>
       </c>
     </row>
-    <row r="210" spans="3:7" hidden="1">
+    <row r="210" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C210">
         <f t="shared" si="5"/>
         <v>150</v>
@@ -8659,7 +8711,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V20');</v>
       </c>
     </row>
-    <row r="211" spans="3:7" hidden="1">
+    <row r="211" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C211">
         <f t="shared" si="5"/>
         <v>151</v>
@@ -8675,7 +8727,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V15/65');</v>
       </c>
     </row>
-    <row r="212" spans="3:7" hidden="1">
+    <row r="212" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C212">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -8691,7 +8743,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V90-3.0');</v>
       </c>
     </row>
-    <row r="213" spans="3:7" hidden="1">
+    <row r="213" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C213">
         <f t="shared" si="5"/>
         <v>153</v>
@@ -8707,7 +8759,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V100-2.0');</v>
       </c>
     </row>
-    <row r="214" spans="3:7" hidden="1">
+    <row r="214" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C214">
         <f t="shared" si="5"/>
         <v>154</v>
@@ -8723,7 +8775,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V42-600');</v>
       </c>
     </row>
-    <row r="215" spans="3:7" hidden="1">
+    <row r="215" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C215">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -8739,7 +8791,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V90-1.8');</v>
       </c>
     </row>
-    <row r="216" spans="3:7" hidden="1">
+    <row r="216" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C216">
         <f t="shared" si="5"/>
         <v>156</v>
@@ -8755,7 +8807,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V112-3.3');</v>
       </c>
     </row>
-    <row r="217" spans="3:7" hidden="1">
+    <row r="217" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C217">
         <f t="shared" si="5"/>
         <v>157</v>
@@ -8771,7 +8823,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM72/1650');</v>
       </c>
     </row>
-    <row r="218" spans="3:7" hidden="1">
+    <row r="218" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C218">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -8787,7 +8839,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M65/13');</v>
       </c>
     </row>
-    <row r="219" spans="3:7" hidden="1">
+    <row r="219" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C219">
         <f t="shared" si="5"/>
         <v>159</v>
@@ -8803,7 +8855,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NedWind');</v>
       </c>
     </row>
-    <row r="220" spans="3:7" hidden="1">
+    <row r="220" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C220">
         <f t="shared" si="5"/>
         <v>160</v>
@@ -8819,7 +8871,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17E');</v>
       </c>
     </row>
-    <row r="221" spans="3:7" hidden="1">
+    <row r="221" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C221">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -8835,7 +8887,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17 ');</v>
       </c>
     </row>
-    <row r="222" spans="3:7" hidden="1">
+    <row r="222" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C222">
         <f t="shared" si="5"/>
         <v>162</v>
@@ -8851,7 +8903,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V112-3.0');</v>
       </c>
     </row>
-    <row r="223" spans="3:7" hidden="1">
+    <row r="223" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C223">
         <f t="shared" si="5"/>
         <v>163</v>
@@ -8867,7 +8919,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V80-2.0');</v>
       </c>
     </row>
-    <row r="224" spans="3:7" hidden="1">
+    <row r="224" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C224">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -8883,7 +8935,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM82/1500');</v>
       </c>
     </row>
-    <row r="225" spans="3:7" hidden="1">
+    <row r="225" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C225">
         <f t="shared" si="5"/>
         <v>165</v>
@@ -8899,7 +8951,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V110-2.0');</v>
       </c>
     </row>
-    <row r="226" spans="3:7" hidden="1">
+    <row r="226" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C226">
         <f t="shared" si="5"/>
         <v>166</v>
@@ -8915,7 +8967,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V15');</v>
       </c>
     </row>
-    <row r="227" spans="3:7" hidden="1">
+    <row r="227" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C227">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -8931,7 +8983,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wincon', 'W200');</v>
       </c>
     </row>
-    <row r="228" spans="3:7" hidden="1">
+    <row r="228" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C228">
         <f t="shared" si="5"/>
         <v>168</v>
@@ -8947,7 +8999,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wincon', 'W99XT');</v>
       </c>
     </row>
-    <row r="229" spans="3:7" hidden="1">
+    <row r="229" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C229">
         <f t="shared" si="5"/>
         <v>169</v>
@@ -8963,7 +9015,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wind Energy Solutions', 'WES 250');</v>
       </c>
     </row>
-    <row r="230" spans="3:7" hidden="1">
+    <row r="230" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C230">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -8979,7 +9031,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmaster', 'Windmaster-211');</v>
       </c>
     </row>
-    <row r="231" spans="3:7" hidden="1">
+    <row r="231" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C231">
         <f t="shared" si="5"/>
         <v>171</v>
@@ -8995,7 +9047,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '17S');</v>
       </c>
     </row>
-    <row r="232" spans="3:7" hidden="1">
+    <row r="232" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C232">
         <f t="shared" si="5"/>
         <v>172</v>
@@ -9011,7 +9063,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '200');</v>
       </c>
     </row>
-    <row r="233" spans="3:7" hidden="1">
+    <row r="233" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C233">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -9027,7 +9079,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '15S');</v>
       </c>
     </row>
-    <row r="240" spans="3:7">
+    <row r="240" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
         <v>360</v>
       </c>
@@ -9035,7 +9087,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="241" spans="4:6">
+    <row r="241" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
         <v>386</v>
       </c>
@@ -9043,7 +9095,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="242" spans="4:6">
+    <row r="242" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
         <v>385</v>
       </c>
@@ -9051,7 +9103,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="243" spans="4:6">
+    <row r="243" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
         <v>367</v>
       </c>
@@ -9059,7 +9111,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="244" spans="4:6">
+    <row r="244" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
         <v>363</v>
       </c>
@@ -9067,7 +9119,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="245" spans="4:6">
+    <row r="245" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
         <v>369</v>
       </c>
@@ -9075,7 +9127,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="246" spans="4:6">
+    <row r="246" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D246" t="s">
         <v>361</v>
       </c>
@@ -9083,7 +9135,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="247" spans="4:6">
+    <row r="247" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
         <v>400</v>
       </c>
@@ -9091,7 +9143,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="248" spans="4:6">
+    <row r="248" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
         <v>366</v>
       </c>
@@ -9099,7 +9151,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="249" spans="4:6">
+    <row r="249" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
         <v>382</v>
       </c>
@@ -9107,7 +9159,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="250" spans="4:6">
+    <row r="250" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
         <v>402</v>
       </c>
@@ -9115,202 +9167,202 @@
         <v>160</v>
       </c>
     </row>
-    <row r="251" spans="4:6">
+    <row r="251" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D251" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="252" spans="4:6">
+    <row r="252" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="253" spans="4:6">
+    <row r="253" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D253" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="254" spans="4:6">
+    <row r="254" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="255" spans="4:6">
+    <row r="255" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="256" spans="4:6">
+    <row r="256" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="257" spans="4:4">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="258" spans="4:4">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D258" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="259" spans="4:4">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D259" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="260" spans="4:4">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D260" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="261" spans="4:4">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D261" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="262" spans="4:4">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D262" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="263" spans="4:4">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D263" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="264" spans="4:4">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D264" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="265" spans="4:4">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D265" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="266" spans="4:4">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="267" spans="4:4">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D267" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="268" spans="4:4">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="269" spans="4:4">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D269" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="270" spans="4:4">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D270" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="271" spans="4:4">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="272" spans="4:4">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="273" spans="4:4">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="274" spans="4:4">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D274" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="275" spans="4:4">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D275" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="276" spans="4:4">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D276" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="277" spans="4:4">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D277" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="278" spans="4:4">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D278" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="279" spans="4:4">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D279" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="280" spans="4:4">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D280" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="281" spans="4:4">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D281" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="282" spans="4:4">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D282" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="283" spans="4:4">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D283" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="284" spans="4:4">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D284" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="285" spans="4:4">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D285" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="286" spans="4:4">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D286" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="287" spans="4:4">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D287" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="288" spans="4:4">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D288" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="289" spans="4:4">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D289" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="290" spans="4:4">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D290" t="s">
         <v>370</v>
       </c>
@@ -9328,10 +9380,5 @@
     <sortCondition ref="D60"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se crea modulo field operations y flight
Se crean modulos y se actualiza db
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="456">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1371,6 +1371,27 @@
   </si>
   <si>
     <t>cada uno.</t>
+  </si>
+  <si>
+    <t>Open /  Closed (Este campo servira para identificar cuando se libere un tecnico de un proyecto)</t>
+  </si>
+  <si>
+    <t>Descripción del vuelo</t>
+  </si>
+  <si>
+    <t>TABLE: FLIGHTS</t>
+  </si>
+  <si>
+    <t>ID FIELD OP</t>
+  </si>
+  <si>
+    <t>ID FLIGHT</t>
+  </si>
+  <si>
+    <t>ID TECH</t>
+  </si>
+  <si>
+    <t>Redundancia para reporte de costo de Tech</t>
   </si>
 </sst>
 </file>
@@ -2269,6 +2290,59 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connector: Elbow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD1AB44A-FAD2-4C84-9E6D-4232800A8E95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="35873531" y="845344"/>
+          <a:ext cx="1047750" cy="761999"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2593,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP60"/>
+  <dimension ref="A1:AS60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AJ21" sqref="AJ21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,9 +2714,12 @@
     <col min="38" max="38" width="19.5703125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
     <col min="40" max="40" width="30.28515625" customWidth="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2684,7 +2761,7 @@
       <c r="AO1" s="2"/>
       <c r="AP1" s="2"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2728,7 +2805,7 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>19</v>
@@ -2787,8 +2864,13 @@
       <c r="AN3" s="2"/>
       <c r="AO3" s="30"/>
       <c r="AP3" s="30"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -2879,8 +2961,17 @@
       </c>
       <c r="AO4" s="29"/>
       <c r="AP4" s="29"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -2963,8 +3054,15 @@
       <c r="AN5" s="32"/>
       <c r="AO5" s="7"/>
       <c r="AP5" s="30"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS5" s="11"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -3043,8 +3141,17 @@
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS6" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -3125,8 +3232,17 @@
       </c>
       <c r="AO7" s="30"/>
       <c r="AP7" s="30"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="AR7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS7" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -3211,8 +3327,17 @@
       </c>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="AR8" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="AS8" s="11" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -3291,8 +3416,15 @@
       </c>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="AR9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS9" s="11"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
         <v>8</v>
@@ -3361,18 +3493,27 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="11" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="AM10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="AN10" s="11" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="AR10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS10" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
@@ -3441,18 +3582,18 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="11" t="s">
-        <v>435</v>
+        <v>39</v>
       </c>
       <c r="AM11" s="11" t="s">
-        <v>436</v>
+        <v>18</v>
       </c>
       <c r="AN11" s="11" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
@@ -3516,19 +3657,13 @@
       </c>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
-      <c r="AL12" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="AM12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="AN12" s="11" t="s">
-        <v>439</v>
-      </c>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -3594,7 +3729,7 @@
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -3648,13 +3783,15 @@
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
+      <c r="AL14" s="2" t="s">
+        <v>447</v>
+      </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -3704,13 +3841,15 @@
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
+      <c r="AL15" s="2" t="s">
+        <v>448</v>
+      </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -3760,9 +3899,7 @@
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
-      <c r="AL16" s="2" t="s">
-        <v>447</v>
-      </c>
+      <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
@@ -3816,9 +3953,7 @@
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
-      <c r="AL17" s="2" t="s">
-        <v>448</v>
-      </c>
+      <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
@@ -4514,9 +4649,6 @@
       <c r="AI32" s="2"/>
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
-      <c r="AL32" s="2"/>
-      <c r="AM32" s="2"/>
-      <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
       <c r="AP32" s="2"/>
     </row>
@@ -4554,9 +4686,6 @@
       <c r="AI33" s="2"/>
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
-      <c r="AL33" s="2"/>
-      <c r="AM33" s="2"/>
-      <c r="AN33" s="2"/>
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Se concluye modulo de fieldop y flights
Se modifica y concluyen los modulos fieldop y flights.
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -19,12 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FIELD VALUES'!$C$60:$E$233</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="464">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1322,9 +1321,6 @@
     <t>PO ASIGNED</t>
   </si>
   <si>
-    <t>BANCH / IN FIELD</t>
-  </si>
-  <si>
     <t>DATA FLIGHT</t>
   </si>
   <si>
@@ -1367,15 +1363,6 @@
     <t xml:space="preserve">Date auto </t>
   </si>
   <si>
-    <t xml:space="preserve">Es necesario definir los perfiles y los niveles de acceso que tendra </t>
-  </si>
-  <si>
-    <t>cada uno.</t>
-  </si>
-  <si>
-    <t>Open /  Closed (Este campo servira para identificar cuando se libere un tecnico de un proyecto)</t>
-  </si>
-  <si>
     <t>Descripción del vuelo</t>
   </si>
   <si>
@@ -1392,6 +1379,42 @@
   </si>
   <si>
     <t>Redundancia para reporte de costo de Tech</t>
+  </si>
+  <si>
+    <t>BANCH / IN FIELD / PENDING  APPROVAL</t>
+  </si>
+  <si>
+    <t>Assigned /  Closed / Pending Approval / Denied (Este campo servira para identificar cuando se libere un tecnico de un proyecto)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed / </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending Approval / </t>
+  </si>
+  <si>
+    <t>Denied</t>
+  </si>
+  <si>
+    <t>Cuando el tecnico se aprueba la asignación a la PO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando al tecnico se libera de la PO </t>
+  </si>
+  <si>
+    <t>Cuando esta pendiente que se apruebe o niegue la participación del tecnico al PO</t>
+  </si>
+  <si>
+    <t>Cuando se niega la participación del tecnico a la PO</t>
+  </si>
+  <si>
+    <t>Cuando nieguen a un tecnico se libera el Tecnico, por lo cual</t>
+  </si>
+  <si>
+    <t>se debera modificar el status de la tabla tecnico pasando a banch</t>
   </si>
 </sst>
 </file>
@@ -2669,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AS11" sqref="AS11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AC1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2888,7 @@
       <c r="AO3" s="30"/>
       <c r="AP3" s="30"/>
       <c r="AQ3" s="3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
@@ -3055,7 +3078,7 @@
       <c r="AO5" s="7"/>
       <c r="AP5" s="30"/>
       <c r="AQ5" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="AR5" s="11" t="s">
         <v>20</v>
@@ -3148,7 +3171,7 @@
         <v>18</v>
       </c>
       <c r="AS6" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
@@ -3228,18 +3251,18 @@
         <v>18</v>
       </c>
       <c r="AN7" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AO7" s="30"/>
       <c r="AP7" s="30"/>
       <c r="AQ7" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AR7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="AS7" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
@@ -3328,13 +3351,13 @@
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
       <c r="AQ8" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="AR8" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="AR8" s="11" t="s">
+      <c r="AS8" s="11" t="s">
         <v>436</v>
-      </c>
-      <c r="AS8" s="11" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
@@ -3412,12 +3435,12 @@
         <v>18</v>
       </c>
       <c r="AN9" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
       <c r="AQ9" s="11" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="AR9" s="11" t="s">
         <v>20</v>
@@ -3488,29 +3511,29 @@
         <v>131</v>
       </c>
       <c r="AI10" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AM10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="AN10" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
       <c r="AQ10" s="11" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="AR10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="AS10" s="11" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
@@ -3574,10 +3597,10 @@
         <v>424</v>
       </c>
       <c r="AH11" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="AI11" s="11" t="s">
         <v>440</v>
-      </c>
-      <c r="AI11" s="11" t="s">
-        <v>441</v>
       </c>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
@@ -3588,7 +3611,7 @@
         <v>18</v>
       </c>
       <c r="AN11" s="11" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
@@ -3653,7 +3676,7 @@
         <v>18</v>
       </c>
       <c r="AI12" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
@@ -3714,7 +3737,7 @@
         <v>18</v>
       </c>
       <c r="AD13" s="35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
@@ -3723,8 +3746,12 @@
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
+      <c r="AL13" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="AM13" s="2" t="s">
+        <v>458</v>
+      </c>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
@@ -3784,9 +3811,11 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="AM14" s="2"/>
+        <v>455</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>459</v>
+      </c>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
@@ -3842,9 +3871,11 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="AM15" s="2"/>
+        <v>456</v>
+      </c>
+      <c r="AM15" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
@@ -3899,8 +3930,12 @@
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="2"/>
+      <c r="AL16" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="2"/>
@@ -4001,7 +4036,9 @@
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
+      <c r="AL18" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
@@ -4049,7 +4086,9 @@
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
-      <c r="AL19" s="2"/>
+      <c r="AL19" s="2" t="s">
+        <v>463</v>
+      </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
@@ -5762,7 +5801,7 @@
         <v>18</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>432</v>
+        <v>452</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Se habilita comentario de rechazo autorizacion (Tecnico y Anticipo)
Se realiza modificación a la base de datos agregando los campos para
guardar los comentarios. Se realiza la modificación de la forma de
desplegar la venta para agregar los comentarios. Se habilita Tooltips
para que se puedan visualizar los mensajes dejados de rechazo solo con
posicionarse donde exista un rechazo
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagarciar\Source\Repos\axis\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="494">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1502,6 +1502,10 @@
   </si>
   <si>
     <t>TABLE: Kit Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+REJECTION COMMENT</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1848,6 +1852,9 @@
     <xf numFmtId="17" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2783,8 +2790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,7 +2832,7 @@
     <col min="35" max="35" width="34.7109375" customWidth="1"/>
     <col min="36" max="36" width="4.7109375" customWidth="1"/>
     <col min="37" max="37" width="4.140625" customWidth="1"/>
-    <col min="38" max="38" width="19.5703125" customWidth="1"/>
+    <col min="38" max="38" width="20.42578125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
     <col min="40" max="40" width="30.28515625" customWidth="1"/>
     <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -3707,7 +3714,7 @@
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
@@ -3771,15 +3778,17 @@
       </c>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
-      <c r="AL12" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
+      <c r="AL12" s="39" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN12" s="11"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -3839,14 +3848,13 @@
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
-      <c r="AL13" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="AM13" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
+      <c r="AL13" s="39" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN13" s="11"/>
       <c r="AP13" s="2"/>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -3904,11 +3912,9 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>458</v>
-      </c>
+        <v>479</v>
+      </c>
+      <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
@@ -3964,10 +3970,10 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>459</v>
+        <v>478</v>
       </c>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
@@ -4026,10 +4032,10 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
@@ -4083,8 +4089,12 @@
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="2"/>
+      <c r="AL17" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>459</v>
+      </c>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
@@ -4132,9 +4142,11 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="AM18" s="2"/>
+        <v>457</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
       <c r="AP18" s="2"/>
@@ -4181,9 +4193,7 @@
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
-      <c r="AL19" s="2" t="s">
-        <v>462</v>
-      </c>
+      <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
@@ -4231,7 +4241,9 @@
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
-      <c r="AL20" s="2"/>
+      <c r="AL20" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
@@ -4281,7 +4293,9 @@
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
-      <c r="AL21" s="2"/>
+      <c r="AL21" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>

</xml_diff>

<commit_message>
Se habilita el la funcion de autorización y cancelación vuelos
Se habilita en el modulo de vuelos la funció de autorización o
cancelación de vuelos con comentarios.
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="498">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1506,6 +1506,19 @@
   <si>
     <t xml:space="preserve">
 REJECTION COMMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Approved /  Pending Approval / Denied (Este campo servira para identificar cuando se libere un tecnico de un proyecto)</t>
+  </si>
+  <si>
+    <t>Cuando esta pendiente que se apruebe o niegue la participación el vuelo</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Cuando se aprueba el vuelo</t>
   </si>
 </sst>
 </file>
@@ -2790,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AQ16" sqref="AQ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,7 +2848,7 @@
     <col min="38" max="38" width="20.42578125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
     <col min="40" max="40" width="30.28515625" customWidth="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3634,7 +3647,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
@@ -3713,6 +3726,15 @@
       </c>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
+      <c r="AQ11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS11" s="39" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="12" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -3787,6 +3809,13 @@
       <c r="AN12" s="11"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
+      <c r="AQ12" s="39" t="s">
+        <v>493</v>
+      </c>
+      <c r="AR12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS12" s="11"/>
     </row>
     <row r="13" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -3918,6 +3947,12 @@
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
+      <c r="AQ14" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -3978,6 +4013,12 @@
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
+      <c r="AQ15" t="s">
+        <v>496</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -4040,6 +4081,9 @@
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="2"/>
+      <c r="AQ16" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
Roles, Usuarios y Correos
Se sube la BD con los datos de los usurios y roles, Son 3 tablas: Roles,
User, UserRoles. Los correos para las pruebas y el excel con los datos
de los usuarios
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="538">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1562,6 +1562,78 @@
   </si>
   <si>
     <t>Asiga a los tecnicos, Actuliza estatus de PO y Contratos</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>no-reply@appsmerida.com</t>
+  </si>
+  <si>
+    <t>pruebamail@appsmerida.com</t>
+  </si>
+  <si>
+    <t>admin@axis.com</t>
+  </si>
+  <si>
+    <t>dhudson@axisrg.com</t>
+  </si>
+  <si>
+    <t>ptattersfield@axisrg.com</t>
+  </si>
+  <si>
+    <t>prueba@axisrg.com</t>
+  </si>
+  <si>
+    <t>gmurrieta@axisrg.com, dalarcon@axisrg.com</t>
+  </si>
+  <si>
+    <t>bmoore@axisrg.com</t>
+  </si>
+  <si>
+    <t>rgallo@axisrg.com</t>
+  </si>
+  <si>
+    <t>bberentson@axisrg.com</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>iprice@axisrg.com; gtapia@axisrg.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Prueba.2017</t>
+  </si>
+  <si>
+    <t>Tecnico.2017</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>AFManager</t>
+  </si>
+  <si>
+    <t>EHSManager</t>
+  </si>
+  <si>
+    <t>RSourceManager</t>
+  </si>
+  <si>
+    <t>AAManager</t>
+  </si>
+  <si>
+    <t>Salesman</t>
+  </si>
+  <si>
+    <t>IdRol</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1643,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1637,6 +1709,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1860,11 +1939,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1914,9 +1997,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1952,7 +2039,7 @@
         <xdr:cNvPr id="3" name="Elbow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2007,7 +2094,7 @@
         <xdr:cNvPr id="5" name="Elbow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2062,7 +2149,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2115,7 +2202,7 @@
         <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2168,7 +2255,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2308,7 @@
         <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2361,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2327,7 +2414,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2380,7 +2467,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2433,7 +2520,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2486,7 +2573,7 @@
         <xdr:cNvPr id="4" name="Connector: Elbow 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD1AB44A-FAD2-4C84-9E6D-4232800A8E95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD1AB44A-FAD2-4C84-9E6D-4232800A8E95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2539,7 +2626,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA8762C4-75E4-4CAA-876C-291079BE25E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA8762C4-75E4-4CAA-876C-291079BE25E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6269,10 +6356,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="C2:R290"/>
+  <dimension ref="C2:W290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6284,12 +6371,17 @@
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" customWidth="1"/>
-    <col min="18" max="18" width="50" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="41.85546875" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" customWidth="1"/>
+    <col min="22" max="22" width="49.5703125" customWidth="1"/>
+    <col min="23" max="23" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:18">
+    <row r="2" spans="4:23">
       <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
@@ -6308,13 +6400,28 @@
         <v>464</v>
       </c>
       <c r="Q2" s="37" t="s">
+        <v>537</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>525</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>527</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="U2" s="37" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="V2" s="37" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="3" spans="4:18">
+      <c r="W2" s="41" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="3" spans="4:23">
       <c r="D3" s="12" t="s">
         <v>58</v>
       </c>
@@ -6332,14 +6439,27 @@
       <c r="P3" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>517</v>
+      </c>
+      <c r="T3" s="43"/>
+      <c r="U3" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="4" spans="4:18">
+      <c r="W3" s="42" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="4" spans="4:23">
       <c r="D4" s="12" t="s">
         <v>58</v>
       </c>
@@ -6356,16 +6476,31 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="P4" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>495</v>
+        <v>469</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="5" spans="4:18">
+        <v>469</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="T4" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="W4" s="43" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="5" spans="4:23">
       <c r="D5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6382,16 +6517,31 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="P5" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>496</v>
+        <v>503</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>4</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="4:18">
+        <v>532</v>
+      </c>
+      <c r="S5" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="T5" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="6" spans="4:23">
       <c r="D6" s="12" t="s">
         <v>58</v>
       </c>
@@ -6407,15 +6557,32 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="P6" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="4:18">
+      <c r="P6" s="40" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q6" s="40">
+        <v>5</v>
+      </c>
+      <c r="R6" s="40" t="s">
+        <v>533</v>
+      </c>
+      <c r="S6" s="42" t="s">
+        <v>524</v>
+      </c>
+      <c r="T6" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U6" s="40" t="s">
+        <v>505</v>
+      </c>
+      <c r="V6" s="40" t="s">
+        <v>507</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="7" spans="4:23">
       <c r="D7" s="12" t="s">
         <v>58</v>
       </c>
@@ -6431,17 +6598,32 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="P7" s="40" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>510</v>
+      <c r="P7" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>6</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="8" spans="4:18">
+        <v>467</v>
+      </c>
+      <c r="S7" s="43" t="s">
+        <v>519</v>
+      </c>
+      <c r="T7" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="8" spans="4:23">
       <c r="D8" s="12" t="s">
         <v>58</v>
       </c>
@@ -6457,17 +6639,32 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="P8" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="9" spans="4:18">
+      <c r="P8" s="40" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q8" s="40">
+        <v>7</v>
+      </c>
+      <c r="R8" s="40" t="s">
+        <v>534</v>
+      </c>
+      <c r="S8" s="42" t="s">
+        <v>521</v>
+      </c>
+      <c r="T8" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="4:23">
       <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
@@ -6483,17 +6680,32 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="P9" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="10" spans="4:18">
+      <c r="P9" s="40" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q9" s="40">
+        <v>8</v>
+      </c>
+      <c r="R9" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="S9" s="42" t="s">
+        <v>523</v>
+      </c>
+      <c r="T9" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U9" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="10" spans="4:23">
       <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
@@ -6509,17 +6721,32 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="P10" s="40" t="s">
-        <v>502</v>
-      </c>
-      <c r="Q10" s="40" t="s">
-        <v>504</v>
+      <c r="P10" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>9</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="11" spans="4:18">
+        <v>536</v>
+      </c>
+      <c r="S10" s="43" t="s">
+        <v>518</v>
+      </c>
+      <c r="T10" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="11" spans="4:23">
       <c r="D11" s="12" t="s">
         <v>58</v>
       </c>
@@ -6535,17 +6762,30 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="P11" s="40" t="s">
-        <v>506</v>
-      </c>
-      <c r="Q11" s="40" t="s">
-        <v>505</v>
-      </c>
-      <c r="R11" s="40" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="12" spans="4:18">
+      <c r="P11" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="S11" s="43" t="s">
+        <v>520</v>
+      </c>
+      <c r="T11" s="43" t="s">
+        <v>530</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="12" spans="4:23">
       <c r="D12" s="12" t="s">
         <v>58</v>
       </c>
@@ -6562,7 +6802,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="4:18">
+    <row r="13" spans="4:23">
       <c r="D13" s="12" t="s">
         <v>58</v>
       </c>
@@ -6579,7 +6819,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="4:18">
+    <row r="14" spans="4:23">
       <c r="D14" s="12" t="s">
         <v>58</v>
       </c>
@@ -6596,7 +6836,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="4:18">
+    <row r="15" spans="4:23">
       <c r="D15" s="12" t="s">
         <v>58</v>
       </c>
@@ -6613,7 +6853,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="4:18">
+    <row r="16" spans="4:23">
       <c r="D16" s="12" t="s">
         <v>58</v>
       </c>
@@ -10055,7 +10295,18 @@
   <sortState ref="D61:E233">
     <sortCondition ref="D60"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="W3" r:id="rId1"/>
+    <hyperlink ref="S3" r:id="rId2"/>
+    <hyperlink ref="S10" r:id="rId3"/>
+    <hyperlink ref="S7" r:id="rId4"/>
+    <hyperlink ref="S11" r:id="rId5"/>
+    <hyperlink ref="S8" r:id="rId6" display="gmurrieta@axisrg.com"/>
+    <hyperlink ref="S5" r:id="rId7"/>
+    <hyperlink ref="S9" r:id="rId8"/>
+    <hyperlink ref="S6" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Asignacion de herramientas y tabla
Se crea el modulo de herramientas
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="465" yWindow="615" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="465" yWindow="615" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FIELD VALUES'!$C$60:$E$233</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="550">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1634,16 +1640,53 @@
   </si>
   <si>
     <t>IdRol</t>
+  </si>
+  <si>
+    <t>TABLE: ASSIGNMENT OF TOOLS</t>
+  </si>
+  <si>
+    <t>AssigmentToolId</t>
+  </si>
+  <si>
+    <t>Supplied by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner, PURCHASE REQUEST TO , RENT (invoice , Cost), SELECT INVENTORY ASSET 
+</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>El costo de la renta o la compra</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Esta campo se activa se se realiza una orden de compra o renta</t>
+  </si>
+  <si>
+    <t>Order Number</t>
+  </si>
+  <si>
+    <t>PurchaseOrderId</t>
+  </si>
+  <si>
+    <t>Relacion con PO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1941,13 +1984,13 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1966,10 +2009,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -2000,6 +2043,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2039,7 +2088,7 @@
         <xdr:cNvPr id="3" name="Elbow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2094,7 +2143,7 @@
         <xdr:cNvPr id="5" name="Elbow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2149,7 +2198,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2202,7 +2251,7 @@
         <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2255,7 +2304,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2308,7 +2357,7 @@
         <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2361,7 +2410,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2414,7 +2463,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2467,7 +2516,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2520,7 +2569,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2573,7 +2622,7 @@
         <xdr:cNvPr id="4" name="Connector: Elbow 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD1AB44A-FAD2-4C84-9E6D-4232800A8E95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD1AB44A-FAD2-4C84-9E6D-4232800A8E95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2626,7 +2675,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA8762C4-75E4-4CAA-876C-291079BE25E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA8762C4-75E4-4CAA-876C-291079BE25E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2636,6 +2685,112 @@
         <a:xfrm>
           <a:off x="8060531" y="13787437"/>
           <a:ext cx="381000" cy="726282"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>33338</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>416718</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EB1A7FE-85B1-40C1-82DE-6984A8D635A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3259932" y="2809875"/>
+          <a:ext cx="23576755" cy="16583026"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>261938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>154781</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967EE2BB-7F67-44F5-B8E5-22CBD2DBE390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8048625" y="2750344"/>
+          <a:ext cx="18526125" cy="11965782"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2707,7 +2862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2739,9 +2894,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2773,6 +2946,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2948,14 +3139,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69:O73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -3001,7 +3192,7 @@
     <col min="45" max="45" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3043,7 +3234,7 @@
       <c r="AO1" s="2"/>
       <c r="AP1" s="2"/>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3087,7 +3278,7 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>19</v>
@@ -3152,7 +3343,7 @@
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>0</v>
@@ -3253,7 +3444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>37</v>
@@ -3344,7 +3535,7 @@
       </c>
       <c r="AS5" s="11"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -3433,7 +3624,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -3524,7 +3715,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -3619,7 +3810,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -3706,7 +3897,7 @@
       </c>
       <c r="AS9" s="11"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
         <v>8</v>
@@ -3795,7 +3986,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:45" ht="45.75">
+    <row r="11" spans="1:45" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>9</v>
@@ -3884,7 +4075,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:45" ht="23.25">
+    <row r="12" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>10</v>
@@ -3965,7 +4156,7 @@
       </c>
       <c r="AS12" s="11"/>
     </row>
-    <row r="13" spans="1:45" ht="23.25">
+    <row r="13" spans="1:45" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -4034,7 +4225,7 @@
       <c r="AN13" s="11"/>
       <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -4102,7 +4293,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>14</v>
@@ -4168,7 +4359,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
@@ -4233,7 +4424,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -4291,7 +4482,7 @@
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4343,7 +4534,7 @@
       <c r="AO18" s="2"/>
       <c r="AP18" s="2"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -4391,7 +4582,7 @@
       <c r="AO19" s="2"/>
       <c r="AP19" s="2"/>
     </row>
-    <row r="20" spans="1:42">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4441,7 +4632,7 @@
       <c r="AO20" s="2"/>
       <c r="AP20" s="2"/>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4493,7 +4684,7 @@
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4543,7 +4734,7 @@
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4593,7 +4784,7 @@
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4643,7 +4834,7 @@
       <c r="AO24" s="2"/>
       <c r="AP24" s="2"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4687,7 +4878,7 @@
       <c r="AO25" s="2"/>
       <c r="AP25" s="2"/>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4731,7 +4922,7 @@
       <c r="AO26" s="2"/>
       <c r="AP26" s="2"/>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4775,7 +4966,7 @@
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4819,7 +5010,7 @@
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4863,7 +5054,7 @@
       <c r="AO29" s="2"/>
       <c r="AP29" s="2"/>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4907,7 +5098,7 @@
       <c r="AO30" s="2"/>
       <c r="AP30" s="2"/>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4951,7 +5142,7 @@
       <c r="AO31" s="2"/>
       <c r="AP31" s="2"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4992,7 +5183,7 @@
       <c r="AO32" s="2"/>
       <c r="AP32" s="2"/>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -5029,7 +5220,7 @@
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
     </row>
-    <row r="34" spans="1:42">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
         <v>77</v>
@@ -5067,7 +5258,7 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row r="35" spans="1:42">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>0</v>
@@ -5126,7 +5317,7 @@
       <c r="Z35" s="29"/>
       <c r="AC35" s="29"/>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
         <v>82</v>
@@ -5184,7 +5375,7 @@
       </c>
       <c r="Z36" s="30"/>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
@@ -5240,7 +5431,7 @@
       </c>
       <c r="Z37" s="30"/>
     </row>
-    <row r="38" spans="1:42">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="6" t="s">
         <v>4</v>
@@ -5296,7 +5487,7 @@
       </c>
       <c r="Z38" s="30"/>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="6" t="s">
         <v>5</v>
@@ -5352,7 +5543,7 @@
       </c>
       <c r="Z39" s="30"/>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="6" t="s">
         <v>76</v>
@@ -5408,7 +5599,7 @@
       </c>
       <c r="Z40" s="30"/>
     </row>
-    <row r="41" spans="1:42">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="6" t="s">
         <v>134</v>
@@ -5468,7 +5659,7 @@
       </c>
       <c r="Z41" s="30"/>
     </row>
-    <row r="42" spans="1:42">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="6" t="s">
         <v>135</v>
@@ -5519,7 +5710,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="6" t="s">
         <v>14</v>
@@ -5564,7 +5755,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="6" t="s">
         <v>136</v>
@@ -5609,7 +5800,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:42">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="6" t="s">
         <v>16</v>
@@ -5654,7 +5845,7 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="6" t="s">
         <v>62</v>
@@ -5699,7 +5890,7 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="6" t="s">
         <v>63</v>
@@ -5744,7 +5935,7 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:42">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="6" t="s">
         <v>64</v>
@@ -5789,7 +5980,7 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="6" t="s">
         <v>66</v>
@@ -5832,7 +6023,7 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="6" t="s">
         <v>73</v>
@@ -5875,7 +6066,7 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="6" t="s">
         <v>67</v>
@@ -5909,7 +6100,7 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="6" t="s">
         <v>74</v>
@@ -5946,7 +6137,7 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
@@ -5977,7 +6168,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="6" t="s">
         <v>69</v>
@@ -6010,7 +6201,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="6" t="s">
         <v>70</v>
@@ -6038,7 +6229,7 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="6" t="s">
         <v>71</v>
@@ -6066,7 +6257,7 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="6" t="s">
         <v>72</v>
@@ -6094,7 +6285,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58" s="31" t="s">
         <v>39</v>
       </c>
@@ -6114,7 +6305,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B59" s="31" t="s">
         <v>431</v>
       </c>
@@ -6132,7 +6323,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:22">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M60" s="8" t="s">
         <v>128</v>
       </c>
@@ -6143,7 +6334,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="2:15" ht="23.25">
+    <row r="67" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>473</v>
       </c>
@@ -6160,7 +6351,7 @@
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="2:15">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>0</v>
       </c>
@@ -6189,7 +6380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:15">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="32" t="s">
         <v>474</v>
       </c>
@@ -6218,7 +6409,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="2:15">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="31" t="s">
         <v>475</v>
       </c>
@@ -6241,7 +6432,7 @@
       </c>
       <c r="O70" s="31"/>
     </row>
-    <row r="71" spans="2:15">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="31" t="s">
         <v>476</v>
       </c>
@@ -6264,7 +6455,7 @@
       </c>
       <c r="O71" s="31"/>
     </row>
-    <row r="72" spans="2:15">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="31" t="s">
         <v>481</v>
       </c>
@@ -6287,7 +6478,7 @@
       </c>
       <c r="O72" s="31"/>
     </row>
-    <row r="73" spans="2:15">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="31" t="s">
         <v>472</v>
       </c>
@@ -6310,14 +6501,25 @@
       <c r="N73" s="31"/>
       <c r="O73" s="31"/>
     </row>
-    <row r="78" spans="2:15">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H74" s="46" t="s">
+        <v>548</v>
+      </c>
+      <c r="I74" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="J74" s="47" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>490</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="2:15">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>0</v>
       </c>
@@ -6328,7 +6530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="2:15">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="32" t="s">
         <v>491</v>
       </c>
@@ -6337,7 +6539,7 @@
       </c>
       <c r="D80" s="32"/>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="31" t="s">
         <v>475</v>
       </c>
@@ -6345,6 +6547,84 @@
         <v>18</v>
       </c>
       <c r="D81" s="31"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="44" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="40" t="s">
+        <v>539</v>
+      </c>
+      <c r="C87" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="D87" s="40"/>
+    </row>
+    <row r="88" spans="2:4" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="46" t="s">
+        <v>540</v>
+      </c>
+      <c r="C88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="47" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="46" t="s">
+        <v>547</v>
+      </c>
+      <c r="C89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="47" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B90" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="C90" s="46" t="s">
+        <v>543</v>
+      </c>
+      <c r="D90" s="47" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="46" t="s">
+        <v>545</v>
+      </c>
+      <c r="C91" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="47"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="46" t="s">
+        <v>548</v>
+      </c>
+      <c r="C92" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="D92" s="47" t="s">
+        <v>549</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6354,15 +6634,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="C2:W290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
@@ -6381,7 +6661,7 @@
     <col min="23" max="23" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:23">
+    <row r="2" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
@@ -6421,7 +6701,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="4:23">
+    <row r="3" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
         <v>58</v>
       </c>
@@ -6459,7 +6739,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="4" spans="4:23">
+    <row r="4" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D4" s="12" t="s">
         <v>58</v>
       </c>
@@ -6500,7 +6780,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="5" spans="4:23">
+    <row r="5" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6541,7 +6821,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="6" spans="4:23">
+    <row r="6" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D6" s="12" t="s">
         <v>58</v>
       </c>
@@ -6582,7 +6862,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="4:23">
+    <row r="7" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>58</v>
       </c>
@@ -6623,7 +6903,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="8" spans="4:23">
+    <row r="8" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>58</v>
       </c>
@@ -6664,7 +6944,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="9" spans="4:23">
+    <row r="9" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
@@ -6705,7 +6985,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="10" spans="4:23">
+    <row r="10" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
@@ -6746,7 +7026,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="4:23">
+    <row r="11" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D11" s="12" t="s">
         <v>58</v>
       </c>
@@ -6785,7 +7065,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="4:23">
+    <row r="12" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D12" s="12" t="s">
         <v>58</v>
       </c>
@@ -6802,7 +7082,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="4:23">
+    <row r="13" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D13" s="12" t="s">
         <v>58</v>
       </c>
@@ -6819,7 +7099,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="4:23">
+    <row r="14" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D14" s="12" t="s">
         <v>58</v>
       </c>
@@ -6836,7 +7116,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="4:23">
+    <row r="15" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D15" s="12" t="s">
         <v>58</v>
       </c>
@@ -6853,7 +7133,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="4:23">
+    <row r="16" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>58</v>
       </c>
@@ -6870,7 +7150,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="4:13">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" s="13" t="s">
         <v>59</v>
       </c>
@@ -6887,7 +7167,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="4:13">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" s="13" t="s">
         <v>59</v>
       </c>
@@ -6904,7 +7184,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="4:13">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D19" s="13" t="s">
         <v>59</v>
       </c>
@@ -6921,7 +7201,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="4:13">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D20" s="13" t="s">
         <v>59</v>
       </c>
@@ -6938,7 +7218,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="4:13">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D21" s="13" t="s">
         <v>59</v>
       </c>
@@ -6955,7 +7235,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="4:13">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" s="13" t="s">
         <v>59</v>
       </c>
@@ -6964,7 +7244,7 @@
         <v>CONSTRUCT: COMMISION</v>
       </c>
     </row>
-    <row r="23" spans="4:13">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D23" s="13" t="s">
         <v>59</v>
       </c>
@@ -6973,7 +7253,7 @@
         <v>CONSTRUCT: OPEN</v>
       </c>
     </row>
-    <row r="26" spans="4:13">
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D26" s="14" t="s">
         <v>149</v>
       </c>
@@ -6981,73 +7261,73 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="4:13">
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="4:13">
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="4:13">
+    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="4:13">
+    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="4:13">
+    <row r="31" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="4:13">
+    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="4:11">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="4:11">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="4:11">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="4:11">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="4:11">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="4:11" ht="15.75" thickBot="1">
+    <row r="42" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>162</v>
       </c>
@@ -7055,7 +7335,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="4:11" ht="24.75" thickBot="1">
+    <row r="43" spans="4:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D43" s="15" t="s">
         <v>49</v>
       </c>
@@ -7069,7 +7349,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="4:11">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="16" t="s">
         <v>167</v>
       </c>
@@ -7081,7 +7361,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="4:11">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="20" t="s">
         <v>168</v>
       </c>
@@ -7093,7 +7373,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="4:11">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="20" t="s">
         <v>165</v>
       </c>
@@ -7103,7 +7383,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="4:11">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="20" t="s">
         <v>165</v>
       </c>
@@ -7113,7 +7393,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="4:11">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="20" t="s">
         <v>171</v>
       </c>
@@ -7125,7 +7405,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="49" spans="3:7">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D49" s="20" t="s">
         <v>172</v>
       </c>
@@ -7137,7 +7417,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="50" spans="3:7">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D50" s="20" t="s">
         <v>173</v>
       </c>
@@ -7147,7 +7427,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="22"/>
     </row>
-    <row r="51" spans="3:7">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D51" s="20" t="s">
         <v>174</v>
       </c>
@@ -7157,7 +7437,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="22"/>
     </row>
-    <row r="52" spans="3:7">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D52" s="20" t="s">
         <v>175</v>
       </c>
@@ -7167,7 +7447,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="3:7">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D53" s="20" t="s">
         <v>176</v>
       </c>
@@ -7177,7 +7457,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="22"/>
     </row>
-    <row r="54" spans="3:7">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D54" s="20" t="s">
         <v>178</v>
       </c>
@@ -7187,7 +7467,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="3:7">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D55" s="20" t="s">
         <v>179</v>
       </c>
@@ -7197,7 +7477,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="3:7">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D56" s="20" t="s">
         <v>180</v>
       </c>
@@ -7207,7 +7487,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="22"/>
     </row>
-    <row r="57" spans="3:7" ht="15.75" thickBot="1">
+    <row r="57" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="23" t="s">
         <v>181</v>
       </c>
@@ -7217,7 +7497,7 @@
       <c r="F57" s="24"/>
       <c r="G57" s="25"/>
     </row>
-    <row r="60" spans="3:7">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>405</v>
       </c>
@@ -7228,7 +7508,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="61" spans="3:7" hidden="1">
+    <row r="61" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" s="28">
         <v>1</v>
       </c>
@@ -7243,7 +7523,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('AAER', 'A1500-77');</v>
       </c>
     </row>
-    <row r="62" spans="3:7" hidden="1">
+    <row r="62" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" s="28">
         <f>+C61+1</f>
         <v>2</v>
@@ -7259,7 +7539,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('AAER', 'A1500-70');</v>
       </c>
     </row>
-    <row r="63" spans="3:7" hidden="1">
+    <row r="63" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" s="28">
         <f t="shared" ref="C63:C126" si="1">+C62+1</f>
         <v>3</v>
@@ -7275,7 +7555,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW3000-116');</v>
       </c>
     </row>
-    <row r="64" spans="3:7" hidden="1">
+    <row r="64" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" s="28">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -7291,7 +7571,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW3000-109');</v>
       </c>
     </row>
-    <row r="65" spans="3:7" hidden="1">
+    <row r="65" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C65" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -7307,7 +7587,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW1500-82');</v>
       </c>
     </row>
-    <row r="66" spans="3:7" hidden="1">
+    <row r="66" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C66" s="28">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -7323,7 +7603,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Acciona', 'AW1500-77');</v>
       </c>
     </row>
-    <row r="67" spans="3:7" hidden="1">
+    <row r="67" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C67" s="28">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -7339,7 +7619,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeroman', 'Aeroman 14.8');</v>
       </c>
     </row>
-    <row r="68" spans="3:7" hidden="1">
+    <row r="68" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" s="28">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -7355,7 +7635,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeronautica', 'Aeronautic 47');</v>
       </c>
     </row>
-    <row r="69" spans="3:7" hidden="1">
+    <row r="69" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C69" s="28">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -7371,7 +7651,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Aeronautica', 'A54-750');</v>
       </c>
     </row>
-    <row r="70" spans="3:7" hidden="1">
+    <row r="70" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C70" s="28">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -7387,7 +7667,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Alstom', 'ECO100');</v>
       </c>
     </row>
-    <row r="71" spans="3:7" hidden="1">
+    <row r="71" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" s="28">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -7403,7 +7683,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Alstom', 'ECO86');</v>
       </c>
     </row>
-    <row r="72" spans="3:7" hidden="1">
+    <row r="72" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" s="28">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -7419,7 +7699,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Atlantic Orient', 'AOC 15/50');</v>
       </c>
     </row>
-    <row r="73" spans="3:7">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="28">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -7435,7 +7715,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Bergey Windpower', 'XL50');</v>
       </c>
     </row>
-    <row r="74" spans="3:7" hidden="1">
+    <row r="74" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74" s="28">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -7451,7 +7731,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('CCWE', 'CCWE-3600D/115');</v>
       </c>
     </row>
-    <row r="75" spans="3:7" hidden="1">
+    <row r="75" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C75" s="28">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -7467,7 +7747,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-96');</v>
       </c>
     </row>
-    <row r="76" spans="3:7" hidden="1">
+    <row r="76" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="28">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -7483,7 +7763,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-93');</v>
       </c>
     </row>
-    <row r="77" spans="3:7" hidden="1">
+    <row r="77" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C77" s="28">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -7499,7 +7779,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Clipper', 'Liberty 2.5-89');</v>
       </c>
     </row>
-    <row r="78" spans="3:7" hidden="1">
+    <row r="78" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C78" s="28">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -7515,7 +7795,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Daewoo Dewind', 'D8.2');</v>
       </c>
     </row>
-    <row r="79" spans="3:7" hidden="1">
+    <row r="79" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C79" s="28">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -7531,7 +7811,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Daewoo Dewind', 'D9.2');</v>
       </c>
     </row>
-    <row r="80" spans="3:7" hidden="1">
+    <row r="80" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C80" s="28">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -7547,7 +7827,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Danwin', '23 E2');</v>
       </c>
     </row>
-    <row r="81" spans="3:7" hidden="1">
+    <row r="81" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C81" s="28">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -7563,7 +7843,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Danwin', '24/160');</v>
       </c>
     </row>
-    <row r="82" spans="3:7" hidden="1">
+    <row r="82" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C82" s="28">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -7579,7 +7859,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('DES', 'Northwind 100');</v>
       </c>
     </row>
-    <row r="83" spans="3:7" hidden="1">
+    <row r="83" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C83" s="28">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -7595,7 +7875,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Eastern Wind Power', 'Sky Farm 50kW VAWT');</v>
       </c>
     </row>
-    <row r="84" spans="3:7" hidden="1">
+    <row r="84" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" s="28">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -7611,7 +7891,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Elecon', 'T600-48');</v>
       </c>
     </row>
-    <row r="85" spans="3:7" hidden="1">
+    <row r="85" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C85" s="28">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -7627,7 +7907,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Elecon', 'T600-48DS');</v>
       </c>
     </row>
-    <row r="86" spans="3:7" hidden="1">
+    <row r="86" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C86" s="28">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -7643,7 +7923,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Endurance', 'E3120 50kW');</v>
       </c>
     </row>
-    <row r="87" spans="3:7" hidden="1">
+    <row r="87" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C87" s="28">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -7659,7 +7939,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Enertech', 'E48');</v>
       </c>
     </row>
-    <row r="88" spans="3:7" hidden="1">
+    <row r="88" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C88" s="28">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -7675,7 +7955,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Enertech', 'Enertech 44/40');</v>
       </c>
     </row>
-    <row r="89" spans="3:7" hidden="1">
+    <row r="89" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C89" s="28">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -7691,7 +7971,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW54-900');</v>
       </c>
     </row>
-    <row r="90" spans="3:7" hidden="1">
+    <row r="90" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C90" s="28">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -7707,7 +7987,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW52-750');</v>
       </c>
     </row>
-    <row r="91" spans="3:7" hidden="1">
+    <row r="91" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C91" s="28">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -7723,7 +8003,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('EWT', 'DW52-900');</v>
       </c>
     </row>
-    <row r="92" spans="3:7" hidden="1">
+    <row r="92" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C92" s="28">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -7739,7 +8019,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL1500');</v>
       </c>
     </row>
-    <row r="93" spans="3:7" hidden="1">
+    <row r="93" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C93" s="28">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -7755,7 +8035,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL100');</v>
       </c>
     </row>
-    <row r="94" spans="3:7" hidden="1">
+    <row r="94" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C94" s="28">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -7771,7 +8051,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL250');</v>
       </c>
     </row>
-    <row r="95" spans="3:7" hidden="1">
+    <row r="95" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C95" s="28">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -7787,7 +8067,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Fuhrländer', 'FL2500/90');</v>
       </c>
     </row>
-    <row r="96" spans="3:7" hidden="1">
+    <row r="96" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C96" s="28">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -7803,7 +8083,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G97-2.0');</v>
       </c>
     </row>
-    <row r="97" spans="3:7" hidden="1">
+    <row r="97" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C97" s="28">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -7819,7 +8099,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G90-2.0');</v>
       </c>
     </row>
-    <row r="98" spans="3:7" hidden="1">
+    <row r="98" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C98" s="28">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -7835,7 +8115,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G52-850');</v>
       </c>
     </row>
-    <row r="99" spans="3:7" hidden="1">
+    <row r="99" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C99" s="28">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -7851,7 +8131,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G87-2.0');</v>
       </c>
     </row>
-    <row r="100" spans="3:7" hidden="1">
+    <row r="100" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C100" s="28">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -7867,7 +8147,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G58-850');</v>
       </c>
     </row>
-    <row r="101" spans="3:7" hidden="1">
+    <row r="101" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C101" s="28">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -7883,7 +8163,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G114-2.0');</v>
       </c>
     </row>
-    <row r="102" spans="3:7" hidden="1">
+    <row r="102" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C102" s="28">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -7899,7 +8179,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G83-2.0');</v>
       </c>
     </row>
-    <row r="103" spans="3:7" hidden="1">
+    <row r="103" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C103" s="28">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -7915,7 +8195,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Gamesa', 'G80-2.0');</v>
       </c>
     </row>
-    <row r="104" spans="3:7">
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C104" s="28">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -7931,7 +8211,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.6 XLE');</v>
       </c>
     </row>
-    <row r="105" spans="3:7">
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C105" s="28">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -7947,7 +8227,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SLE');</v>
       </c>
     </row>
-    <row r="106" spans="3:7">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C106" s="28">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -7963,7 +8243,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.85-82.5');</v>
       </c>
     </row>
-    <row r="107" spans="3:7">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" s="28">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -7979,7 +8259,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.6-100');</v>
       </c>
     </row>
-    <row r="108" spans="3:7">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="28">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -7995,7 +8275,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 XLE');</v>
       </c>
     </row>
-    <row r="109" spans="3:7">
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="28">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -8011,7 +8291,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.85-87');</v>
       </c>
     </row>
-    <row r="110" spans="3:7">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C110" s="28">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -8027,7 +8307,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-50');</v>
       </c>
     </row>
-    <row r="111" spans="3:7">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C111" s="28">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -8043,7 +8323,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.68-82.5');</v>
       </c>
     </row>
-    <row r="112" spans="3:7">
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C112" s="28">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -8059,7 +8339,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 S');</v>
       </c>
     </row>
-    <row r="113" spans="3:7">
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C113" s="28">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -8075,7 +8355,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.85-103');</v>
       </c>
     </row>
-    <row r="114" spans="3:7">
+    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C114" s="28">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -8091,7 +8371,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.5-120');</v>
       </c>
     </row>
-    <row r="115" spans="3:7">
+    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C115" s="28">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -8107,7 +8387,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.7-100');</v>
       </c>
     </row>
-    <row r="116" spans="3:7">
+    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" s="28">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -8123,7 +8403,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.7-103');</v>
       </c>
     </row>
-    <row r="117" spans="3:7">
+    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" s="28">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -8139,7 +8419,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-40');</v>
       </c>
     </row>
-    <row r="118" spans="3:7">
+    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C118" s="28">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -8155,7 +8435,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5SL');</v>
       </c>
     </row>
-    <row r="119" spans="3:7">
+    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C119" s="28">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -8171,7 +8451,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', '1.5s (Enron)');</v>
       </c>
     </row>
-    <row r="120" spans="3:7">
+    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C120" s="28">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -8187,7 +8467,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SE');</v>
       </c>
     </row>
-    <row r="121" spans="3:7">
+    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C121" s="28">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -8203,7 +8483,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 2.5-100');</v>
       </c>
     </row>
-    <row r="122" spans="3:7">
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C122" s="28">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -8219,7 +8499,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'GE 1.5 SL');</v>
       </c>
     </row>
-    <row r="123" spans="3:7">
+    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C123" s="28">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -8235,7 +8515,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('GE', 'Z-48');</v>
       </c>
     </row>
-    <row r="124" spans="3:7" hidden="1">
+    <row r="124" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C124" s="28">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -8251,7 +8531,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW82');</v>
       </c>
     </row>
-    <row r="125" spans="3:7" hidden="1">
+    <row r="125" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C125" s="28">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -8267,7 +8547,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW87');</v>
       </c>
     </row>
-    <row r="126" spans="3:7" hidden="1">
+    <row r="126" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C126" s="28">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -8283,7 +8563,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW100-2.5');</v>
       </c>
     </row>
-    <row r="127" spans="3:7" hidden="1">
+    <row r="127" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C127" s="28">
         <f t="shared" ref="C127:C190" si="3">+C126+1</f>
         <v>67</v>
@@ -8299,7 +8579,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Goldwind', 'GW77');</v>
       </c>
     </row>
-    <row r="128" spans="3:7" hidden="1">
+    <row r="128" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C128" s="28">
         <f t="shared" si="3"/>
         <v>68</v>
@@ -8315,7 +8595,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('HHI', 'HQ2000');</v>
       </c>
     </row>
-    <row r="129" spans="3:7" hidden="1">
+    <row r="129" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C129" s="28">
         <f t="shared" si="3"/>
         <v>69</v>
@@ -8331,7 +8611,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('HHI', 'HQ1650');</v>
       </c>
     </row>
-    <row r="130" spans="3:7" hidden="1">
+    <row r="130" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C130" s="28">
         <f t="shared" si="3"/>
         <v>70</v>
@@ -8347,7 +8627,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Jonica Impianti', 'JIMP25');</v>
       </c>
     </row>
-    <row r="131" spans="3:7" hidden="1">
+    <row r="131" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C131" s="28">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -8363,7 +8643,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Kenersys', 'K100');</v>
       </c>
     </row>
-    <row r="132" spans="3:7" hidden="1">
+    <row r="132" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C132" s="28">
         <f t="shared" si="3"/>
         <v>72</v>
@@ -8379,7 +8659,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Kenetech', '56-100');</v>
       </c>
     </row>
-    <row r="133" spans="3:7" hidden="1">
+    <row r="133" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C133" s="28">
         <f t="shared" si="3"/>
         <v>73</v>
@@ -8395,7 +8675,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Leitwind', 'LTW77-1.5');</v>
       </c>
     </row>
-    <row r="134" spans="3:7" hidden="1">
+    <row r="134" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C134" s="28">
         <f t="shared" si="3"/>
         <v>74</v>
@@ -8411,7 +8691,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT62/1.0');</v>
       </c>
     </row>
-    <row r="135" spans="3:7" hidden="1">
+    <row r="135" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C135" s="28">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -8427,7 +8707,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-1000');</v>
       </c>
     </row>
-    <row r="136" spans="3:7" hidden="1">
+    <row r="136" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C136" s="28">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -8443,7 +8723,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT92/2.4');</v>
       </c>
     </row>
-    <row r="137" spans="3:7" hidden="1">
+    <row r="137" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C137" s="28">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -8459,7 +8739,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-600');</v>
       </c>
     </row>
-    <row r="138" spans="3:7" hidden="1">
+    <row r="138" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C138" s="28">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -8475,7 +8755,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT95/2.4');</v>
       </c>
     </row>
-    <row r="139" spans="3:7" hidden="1">
+    <row r="139" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C139" s="28">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -8491,7 +8771,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT-250');</v>
       </c>
     </row>
-    <row r="140" spans="3:7" hidden="1">
+    <row r="140" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C140" s="28">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -8507,7 +8787,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT102/2.4');</v>
       </c>
     </row>
-    <row r="141" spans="3:7" hidden="1">
+    <row r="141" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C141" s="28">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -8523,7 +8803,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Mitsubishi', 'MWT100/2.4');</v>
       </c>
     </row>
-    <row r="142" spans="3:7" hidden="1">
+    <row r="142" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C142" s="28">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -8539,7 +8819,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N54/1000');</v>
       </c>
     </row>
-    <row r="143" spans="3:7" hidden="1">
+    <row r="143" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C143" s="28">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -8555,7 +8835,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N43/600');</v>
       </c>
     </row>
-    <row r="144" spans="3:7" hidden="1">
+    <row r="144" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C144" s="28">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -8571,7 +8851,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2300');</v>
       </c>
     </row>
-    <row r="145" spans="3:7" hidden="1">
+    <row r="145" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C145" s="28">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -8587,7 +8867,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N60/1300');</v>
       </c>
     </row>
-    <row r="146" spans="3:7" hidden="1">
+    <row r="146" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C146" s="28">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -8603,7 +8883,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N100/2500');</v>
       </c>
     </row>
-    <row r="147" spans="3:7" hidden="1">
+    <row r="147" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C147" s="28">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -8619,7 +8899,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2500 LS');</v>
       </c>
     </row>
-    <row r="148" spans="3:7" hidden="1">
+    <row r="148" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C148" s="28">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -8635,7 +8915,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N90/2500 HS');</v>
       </c>
     </row>
-    <row r="149" spans="3:7" hidden="1">
+    <row r="149" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C149" s="28">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -8651,7 +8931,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordex', 'N117/2400');</v>
       </c>
     </row>
-    <row r="150" spans="3:7" hidden="1">
+    <row r="150" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C150" s="28">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -8667,7 +8947,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Nordic', 'N1000');</v>
       </c>
     </row>
-    <row r="151" spans="3:7" hidden="1">
+    <row r="151" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C151" s="28">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -8683,7 +8963,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Northern Power Systems', 'NPS 100');</v>
       </c>
     </row>
-    <row r="152" spans="3:7" hidden="1">
+    <row r="152" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C152" s="28">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -8699,7 +8979,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Northern Power Systems', 'NPS Prototype');</v>
       </c>
     </row>
-    <row r="153" spans="3:7" hidden="1">
+    <row r="153" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C153">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -8715,7 +8995,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Pioneer', 'P-1650');</v>
       </c>
     </row>
-    <row r="154" spans="3:7" hidden="1">
+    <row r="154" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C154">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -8731,7 +9011,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('PowerWind', 'PowerWind 56');</v>
       </c>
     </row>
-    <row r="155" spans="3:7" hidden="1">
+    <row r="155" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C155">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -8747,7 +9027,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Renewegy', 'VP-20');</v>
       </c>
     </row>
-    <row r="156" spans="3:7" hidden="1">
+    <row r="156" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C156">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -8763,7 +9043,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('RRB Energy', 'PS-600');</v>
       </c>
     </row>
-    <row r="157" spans="3:7" hidden="1">
+    <row r="157" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C157">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -8779,7 +9059,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE100/2.0');</v>
       </c>
     </row>
-    <row r="158" spans="3:7" hidden="1">
+    <row r="158" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C158">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -8795,7 +9075,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE93/2.0');</v>
       </c>
     </row>
-    <row r="159" spans="3:7" hidden="1">
+    <row r="159" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C159">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -8811,7 +9091,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sany', 'SE8720IIIE');</v>
       </c>
     </row>
-    <row r="160" spans="3:7" hidden="1">
+    <row r="160" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C160">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -8827,7 +9107,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Senvion', 'MM92');</v>
       </c>
     </row>
-    <row r="161" spans="3:7" hidden="1">
+    <row r="161" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C161">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -8843,7 +9123,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('SHI', 'SHI2.5-100');</v>
       </c>
     </row>
-    <row r="162" spans="3:7" hidden="1">
+    <row r="162" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C162">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -8859,7 +9139,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B19/120');</v>
       </c>
     </row>
-    <row r="163" spans="3:7" hidden="1">
+    <row r="163" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C163">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -8875,7 +9155,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-101');</v>
       </c>
     </row>
-    <row r="164" spans="3:7" hidden="1">
+    <row r="164" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C164">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -8891,7 +9171,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B37/450');</v>
       </c>
     </row>
-    <row r="165" spans="3:7" hidden="1">
+    <row r="165" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C165">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -8907,7 +9187,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-93');</v>
       </c>
     </row>
-    <row r="166" spans="3:7" hidden="1">
+    <row r="166" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C166">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -8923,7 +9203,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT3.0-101');</v>
       </c>
     </row>
-    <row r="167" spans="3:7" hidden="1">
+    <row r="167" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C167">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -8939,7 +9219,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT2.3-108');</v>
       </c>
     </row>
-    <row r="168" spans="3:7" hidden="1">
+    <row r="168" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C168">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -8955,7 +9235,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B62/1300');</v>
       </c>
     </row>
-    <row r="169" spans="3:7" hidden="1">
+    <row r="169" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C169">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -8971,7 +9251,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT-2.3');</v>
       </c>
     </row>
-    <row r="170" spans="3:7" hidden="1">
+    <row r="170" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C170">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -8987,7 +9267,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B15/65');</v>
       </c>
     </row>
-    <row r="171" spans="3:7" hidden="1">
+    <row r="171" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C171">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -9003,7 +9283,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'SWT3.0-113');</v>
       </c>
     </row>
-    <row r="172" spans="3:7" hidden="1">
+    <row r="172" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C172">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -9019,7 +9299,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siemens', 'B23/150');</v>
       </c>
     </row>
-    <row r="173" spans="3:7" hidden="1">
+    <row r="173" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C173">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -9035,7 +9315,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sinovel', 'SL 3000/90');</v>
       </c>
     </row>
-    <row r="174" spans="3:7" hidden="1">
+    <row r="174" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C174">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -9051,7 +9331,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Sinovel', 'SL 1500/82');</v>
       </c>
     </row>
-    <row r="175" spans="3:7" hidden="1">
+    <row r="175" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C175">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -9067,7 +9347,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Siva', '250/50');</v>
       </c>
     </row>
-    <row r="176" spans="3:7" hidden="1">
+    <row r="176" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C176">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -9083,7 +9363,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S88-2.1');</v>
       </c>
     </row>
-    <row r="177" spans="3:7" hidden="1">
+    <row r="177" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C177">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -9099,7 +9379,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S64-1.25');</v>
       </c>
     </row>
-    <row r="178" spans="3:7" hidden="1">
+    <row r="178" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C178">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -9115,7 +9395,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S95-2.1');</v>
       </c>
     </row>
-    <row r="179" spans="3:7" hidden="1">
+    <row r="179" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C179">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -9131,7 +9411,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Suzlon', 'S97-2.1');</v>
       </c>
     </row>
-    <row r="180" spans="3:7" hidden="1">
+    <row r="180" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C180">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -9147,7 +9427,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Turbowinds', 'T600-48');</v>
       </c>
     </row>
-    <row r="181" spans="3:7" hidden="1">
+    <row r="181" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C181">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -9163,7 +9443,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Turbowinds', 'T400-34');</v>
       </c>
     </row>
-    <row r="182" spans="3:7" hidden="1">
+    <row r="182" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C182">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -9179,7 +9459,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Unison', 'U54');</v>
       </c>
     </row>
-    <row r="183" spans="3:7" hidden="1">
+    <row r="183" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C183">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -9195,7 +9475,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vanguard', '95T');</v>
       </c>
     </row>
-    <row r="184" spans="3:7" hidden="1">
+    <row r="184" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C184">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -9211,7 +9491,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', 'Vensys 70');</v>
       </c>
     </row>
-    <row r="185" spans="3:7" hidden="1">
+    <row r="185" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C185">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -9227,7 +9507,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', 'Vensys 82');</v>
       </c>
     </row>
-    <row r="186" spans="3:7" hidden="1">
+    <row r="186" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C186">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -9243,7 +9523,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vensys', ' Vensys 77');</v>
       </c>
     </row>
-    <row r="187" spans="3:7" hidden="1">
+    <row r="187" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C187">
         <f t="shared" si="3"/>
         <v>127</v>
@@ -9259,7 +9539,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vergnet', 'MP-R');</v>
       </c>
     </row>
-    <row r="188" spans="3:7" hidden="1">
+    <row r="188" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C188">
         <f t="shared" si="3"/>
         <v>128</v>
@@ -9275,7 +9555,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V27-225');</v>
       </c>
     </row>
-    <row r="189" spans="3:7" hidden="1">
+    <row r="189" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C189">
         <f t="shared" si="3"/>
         <v>129</v>
@@ -9291,7 +9571,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M108/19');</v>
       </c>
     </row>
-    <row r="190" spans="3:7" hidden="1">
+    <row r="190" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C190">
         <f t="shared" si="3"/>
         <v>130</v>
@@ -9307,7 +9587,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM54/950');</v>
       </c>
     </row>
-    <row r="191" spans="3:7" hidden="1">
+    <row r="191" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C191">
         <f t="shared" ref="C191:C233" si="5">+C190+1</f>
         <v>131</v>
@@ -9323,7 +9603,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM52/900');</v>
       </c>
     </row>
-    <row r="192" spans="3:7" hidden="1">
+    <row r="192" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C192">
         <f t="shared" si="5"/>
         <v>132</v>
@@ -9339,7 +9619,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NTK500/37');</v>
       </c>
     </row>
-    <row r="193" spans="3:7" hidden="1">
+    <row r="193" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C193">
         <f t="shared" si="5"/>
         <v>133</v>
@@ -9355,7 +9635,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V42');</v>
       </c>
     </row>
-    <row r="194" spans="3:7" hidden="1">
+    <row r="194" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C194">
         <f t="shared" si="5"/>
         <v>134</v>
@@ -9371,7 +9651,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V47-660');</v>
       </c>
     </row>
-    <row r="195" spans="3:7" hidden="1">
+    <row r="195" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C195">
         <f t="shared" si="5"/>
         <v>135</v>
@@ -9387,7 +9667,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM48/750');</v>
       </c>
     </row>
-    <row r="196" spans="3:7" hidden="1">
+    <row r="196" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C196">
         <f t="shared" si="5"/>
         <v>136</v>
@@ -9403,7 +9683,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V100-1.8');</v>
       </c>
     </row>
-    <row r="197" spans="3:7" hidden="1">
+    <row r="197" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C197">
         <f t="shared" si="5"/>
         <v>137</v>
@@ -9419,7 +9699,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V82-1.65');</v>
       </c>
     </row>
-    <row r="198" spans="3:7" hidden="1">
+    <row r="198" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C198">
         <f t="shared" si="5"/>
         <v>138</v>
@@ -9435,7 +9715,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM82/1650');</v>
       </c>
     </row>
-    <row r="199" spans="3:7" hidden="1">
+    <row r="199" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C199">
         <f t="shared" si="5"/>
         <v>139</v>
@@ -9451,7 +9731,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V44-600');</v>
       </c>
     </row>
-    <row r="200" spans="3:7" hidden="1">
+    <row r="200" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C200">
         <f t="shared" si="5"/>
         <v>140</v>
@@ -9467,7 +9747,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NTK65/17');</v>
       </c>
     </row>
-    <row r="201" spans="3:7" hidden="1">
+    <row r="201" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C201">
         <f t="shared" si="5"/>
         <v>141</v>
@@ -9483,7 +9763,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM44/750');</v>
       </c>
     </row>
-    <row r="202" spans="3:7" hidden="1">
+    <row r="202" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C202">
         <f t="shared" si="5"/>
         <v>142</v>
@@ -9499,7 +9779,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'W250/29');</v>
       </c>
     </row>
-    <row r="203" spans="3:7" hidden="1">
+    <row r="203" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C203">
         <f t="shared" si="5"/>
         <v>143</v>
@@ -9515,7 +9795,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V80-1.8');</v>
       </c>
     </row>
-    <row r="204" spans="3:7" hidden="1">
+    <row r="204" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C204">
         <f t="shared" si="5"/>
         <v>144</v>
@@ -9531,7 +9811,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM950/54');</v>
       </c>
     </row>
-    <row r="205" spans="3:7" hidden="1">
+    <row r="205" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C205">
         <f t="shared" si="5"/>
         <v>145</v>
@@ -9547,7 +9827,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M700/225');</v>
       </c>
     </row>
-    <row r="206" spans="3:7" hidden="1">
+    <row r="206" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C206">
         <f t="shared" si="5"/>
         <v>146</v>
@@ -9563,7 +9843,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM72c/1500');</v>
       </c>
     </row>
-    <row r="207" spans="3:7" hidden="1">
+    <row r="207" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C207">
         <f t="shared" si="5"/>
         <v>147</v>
@@ -9579,7 +9859,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17');</v>
       </c>
     </row>
-    <row r="208" spans="3:7" hidden="1">
+    <row r="208" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C208">
         <f t="shared" si="5"/>
         <v>148</v>
@@ -9595,7 +9875,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V39-500');</v>
       </c>
     </row>
-    <row r="209" spans="3:7" hidden="1">
+    <row r="209" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C209">
         <f t="shared" si="5"/>
         <v>149</v>
@@ -9611,7 +9891,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V27');</v>
       </c>
     </row>
-    <row r="210" spans="3:7" hidden="1">
+    <row r="210" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C210">
         <f t="shared" si="5"/>
         <v>150</v>
@@ -9627,7 +9907,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V20');</v>
       </c>
     </row>
-    <row r="211" spans="3:7" hidden="1">
+    <row r="211" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C211">
         <f t="shared" si="5"/>
         <v>151</v>
@@ -9643,7 +9923,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V15/65');</v>
       </c>
     </row>
-    <row r="212" spans="3:7" hidden="1">
+    <row r="212" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C212">
         <f t="shared" si="5"/>
         <v>152</v>
@@ -9659,7 +9939,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V90-3.0');</v>
       </c>
     </row>
-    <row r="213" spans="3:7" hidden="1">
+    <row r="213" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C213">
         <f t="shared" si="5"/>
         <v>153</v>
@@ -9675,7 +9955,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V100-2.0');</v>
       </c>
     </row>
-    <row r="214" spans="3:7" hidden="1">
+    <row r="214" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C214">
         <f t="shared" si="5"/>
         <v>154</v>
@@ -9691,7 +9971,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V42-600');</v>
       </c>
     </row>
-    <row r="215" spans="3:7" hidden="1">
+    <row r="215" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C215">
         <f t="shared" si="5"/>
         <v>155</v>
@@ -9707,7 +9987,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V90-1.8');</v>
       </c>
     </row>
-    <row r="216" spans="3:7" hidden="1">
+    <row r="216" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C216">
         <f t="shared" si="5"/>
         <v>156</v>
@@ -9723,7 +10003,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V112-3.3');</v>
       </c>
     </row>
-    <row r="217" spans="3:7" hidden="1">
+    <row r="217" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C217">
         <f t="shared" si="5"/>
         <v>157</v>
@@ -9739,7 +10019,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM72/1650');</v>
       </c>
     </row>
-    <row r="218" spans="3:7" hidden="1">
+    <row r="218" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C218">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -9755,7 +10035,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'M65/13');</v>
       </c>
     </row>
-    <row r="219" spans="3:7" hidden="1">
+    <row r="219" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C219">
         <f t="shared" si="5"/>
         <v>159</v>
@@ -9771,7 +10051,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NedWind');</v>
       </c>
     </row>
-    <row r="220" spans="3:7" hidden="1">
+    <row r="220" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C220">
         <f t="shared" si="5"/>
         <v>160</v>
@@ -9787,7 +10067,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17E');</v>
       </c>
     </row>
-    <row r="221" spans="3:7" hidden="1">
+    <row r="221" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C221">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -9803,7 +10083,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V17 ');</v>
       </c>
     </row>
-    <row r="222" spans="3:7" hidden="1">
+    <row r="222" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C222">
         <f t="shared" si="5"/>
         <v>162</v>
@@ -9819,7 +10099,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V112-3.0');</v>
       </c>
     </row>
-    <row r="223" spans="3:7" hidden="1">
+    <row r="223" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C223">
         <f t="shared" si="5"/>
         <v>163</v>
@@ -9835,7 +10115,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V80-2.0');</v>
       </c>
     </row>
-    <row r="224" spans="3:7" hidden="1">
+    <row r="224" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C224">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -9851,7 +10131,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'NM82/1500');</v>
       </c>
     </row>
-    <row r="225" spans="3:7" hidden="1">
+    <row r="225" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C225">
         <f t="shared" si="5"/>
         <v>165</v>
@@ -9867,7 +10147,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V110-2.0');</v>
       </c>
     </row>
-    <row r="226" spans="3:7" hidden="1">
+    <row r="226" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C226">
         <f t="shared" si="5"/>
         <v>166</v>
@@ -9883,7 +10163,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Vestas', 'V15');</v>
       </c>
     </row>
-    <row r="227" spans="3:7" hidden="1">
+    <row r="227" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C227">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -9899,7 +10179,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wincon', 'W200');</v>
       </c>
     </row>
-    <row r="228" spans="3:7" hidden="1">
+    <row r="228" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C228">
         <f t="shared" si="5"/>
         <v>168</v>
@@ -9915,7 +10195,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wincon', 'W99XT');</v>
       </c>
     </row>
-    <row r="229" spans="3:7" hidden="1">
+    <row r="229" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C229">
         <f t="shared" si="5"/>
         <v>169</v>
@@ -9931,7 +10211,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Wind Energy Solutions', 'WES 250');</v>
       </c>
     </row>
-    <row r="230" spans="3:7" hidden="1">
+    <row r="230" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C230">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -9947,7 +10227,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmaster', 'Windmaster-211');</v>
       </c>
     </row>
-    <row r="231" spans="3:7" hidden="1">
+    <row r="231" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C231">
         <f t="shared" si="5"/>
         <v>171</v>
@@ -9963,7 +10243,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '17S');</v>
       </c>
     </row>
-    <row r="232" spans="3:7" hidden="1">
+    <row r="232" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C232">
         <f t="shared" si="5"/>
         <v>172</v>
@@ -9979,7 +10259,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '200');</v>
       </c>
     </row>
-    <row r="233" spans="3:7" hidden="1">
+    <row r="233" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C233">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -9995,7 +10275,7 @@
         <v>INSERT INTO `axisdb`.`platforms` (`ManufactereName`, `PlatformName`) VALUES ('Windmatic', '15S');</v>
       </c>
     </row>
-    <row r="240" spans="3:7">
+    <row r="240" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
         <v>360</v>
       </c>
@@ -10003,7 +10283,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="241" spans="4:6">
+    <row r="241" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
         <v>386</v>
       </c>
@@ -10011,7 +10291,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="242" spans="4:6">
+    <row r="242" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
         <v>385</v>
       </c>
@@ -10019,7 +10299,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="243" spans="4:6">
+    <row r="243" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
         <v>367</v>
       </c>
@@ -10027,7 +10307,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="244" spans="4:6">
+    <row r="244" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
         <v>363</v>
       </c>
@@ -10035,7 +10315,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="245" spans="4:6">
+    <row r="245" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
         <v>369</v>
       </c>
@@ -10043,7 +10323,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="246" spans="4:6">
+    <row r="246" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D246" t="s">
         <v>361</v>
       </c>
@@ -10051,7 +10331,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="247" spans="4:6">
+    <row r="247" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
         <v>400</v>
       </c>
@@ -10059,7 +10339,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="248" spans="4:6">
+    <row r="248" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
         <v>366</v>
       </c>
@@ -10067,7 +10347,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="249" spans="4:6">
+    <row r="249" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
         <v>382</v>
       </c>
@@ -10075,7 +10355,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="250" spans="4:6">
+    <row r="250" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
         <v>402</v>
       </c>
@@ -10083,202 +10363,202 @@
         <v>160</v>
       </c>
     </row>
-    <row r="251" spans="4:6">
+    <row r="251" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D251" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="252" spans="4:6">
+    <row r="252" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="253" spans="4:6">
+    <row r="253" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D253" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="254" spans="4:6">
+    <row r="254" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="255" spans="4:6">
+    <row r="255" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="256" spans="4:6">
+    <row r="256" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="257" spans="4:4">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="258" spans="4:4">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D258" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="259" spans="4:4">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D259" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="260" spans="4:4">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D260" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="261" spans="4:4">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D261" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="262" spans="4:4">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D262" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="263" spans="4:4">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D263" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="264" spans="4:4">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D264" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="265" spans="4:4">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D265" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="266" spans="4:4">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="267" spans="4:4">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D267" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="268" spans="4:4">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="269" spans="4:4">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D269" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="270" spans="4:4">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D270" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="271" spans="4:4">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="272" spans="4:4">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="273" spans="4:4">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="274" spans="4:4">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D274" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="275" spans="4:4">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D275" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="276" spans="4:4">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D276" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="277" spans="4:4">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D277" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="278" spans="4:4">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D278" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="279" spans="4:4">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D279" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="280" spans="4:4">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D280" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="281" spans="4:4">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D281" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="282" spans="4:4">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D282" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="283" spans="4:4">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D283" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="284" spans="4:4">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D284" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="285" spans="4:4">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D285" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="286" spans="4:4">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D286" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="287" spans="4:4">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D287" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="288" spans="4:4">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D288" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="289" spans="4:4">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D289" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="290" spans="4:4">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D290" t="s">
         <v>370</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion Field y ChangeTeches
Se actualizan status de cambio de tecnicos y la vista de liberacion de
tecnico
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="562">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1645,9 +1645,6 @@
     <t>TABLE: ASSIGNMENT OF TOOLS</t>
   </si>
   <si>
-    <t>AssigmentToolId</t>
-  </si>
-  <si>
     <t>Supplied by</t>
   </si>
   <si>
@@ -1677,6 +1674,45 @@
   </si>
   <si>
     <t>Relacion con PO</t>
+  </si>
+  <si>
+    <t>TABLE: TRUCKS</t>
+  </si>
+  <si>
+    <t>NumberTrucks</t>
+  </si>
+  <si>
+    <t>Numero de autos</t>
+  </si>
+  <si>
+    <t>RentaAgency</t>
+  </si>
+  <si>
+    <t>Agencia rentadora de autos</t>
+  </si>
+  <si>
+    <t>El costo de la renta</t>
+  </si>
+  <si>
+    <t>Other1</t>
+  </si>
+  <si>
+    <t>Campo adicional</t>
+  </si>
+  <si>
+    <t>PackingList</t>
+  </si>
+  <si>
+    <t>Lista de envio</t>
+  </si>
+  <si>
+    <t>AirwayBill</t>
+  </si>
+  <si>
+    <t>Costo de envio</t>
+  </si>
+  <si>
+    <t>TABLE: SHIPPINGS</t>
   </si>
 </sst>
 </file>
@@ -3143,7 +3179,7 @@
   <dimension ref="A1:AS92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+      <selection activeCell="M89" sqref="M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6503,13 +6539,13 @@
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H74" s="46" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I74" s="46" t="s">
         <v>439</v>
       </c>
       <c r="J74" s="47" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
@@ -6539,7 +6575,7 @@
       </c>
       <c r="D80" s="32"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="31" t="s">
         <v>475</v>
       </c>
@@ -6548,12 +6584,18 @@
       </c>
       <c r="D81" s="31"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="44" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>549</v>
+      </c>
+      <c r="M85" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="45" t="s">
         <v>0</v>
       </c>
@@ -6563,68 +6605,170 @@
       <c r="D86" s="45" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="40" t="s">
-        <v>539</v>
+      <c r="H86" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="I86" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="M86" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="N86" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="O86" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B87" s="46" t="s">
+        <v>547</v>
       </c>
       <c r="C87" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="D87" s="40"/>
-    </row>
-    <row r="88" spans="2:4" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="D87" s="47" t="s">
+        <v>548</v>
+      </c>
+      <c r="H87" s="46" t="s">
+        <v>547</v>
+      </c>
+      <c r="I87" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="J87" s="47" t="s">
+        <v>548</v>
+      </c>
+      <c r="M87" s="46" t="s">
+        <v>547</v>
+      </c>
+      <c r="N87" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="O87" s="47" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" ht="68.25" x14ac:dyDescent="0.25">
       <c r="B88" s="46" t="s">
+        <v>539</v>
+      </c>
+      <c r="C88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="C88" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D88" s="47" t="s">
+      <c r="H88" s="46" t="s">
+        <v>550</v>
+      </c>
+      <c r="I88" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="J88" s="47" t="s">
+        <v>551</v>
+      </c>
+      <c r="M88" s="46" t="s">
+        <v>557</v>
+      </c>
+      <c r="N88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="47" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="46" t="s">
+        <v>546</v>
+      </c>
+      <c r="C89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="47" t="s">
+        <v>545</v>
+      </c>
+      <c r="H89" s="46" t="s">
+        <v>552</v>
+      </c>
+      <c r="I89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="J89" s="47" t="s">
+        <v>553</v>
+      </c>
+      <c r="M89" s="46" t="s">
+        <v>559</v>
+      </c>
+      <c r="N89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O89" s="47"/>
+    </row>
+    <row r="90" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B90" s="46" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="46" t="s">
-        <v>547</v>
-      </c>
-      <c r="C89" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D89" s="47" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B90" s="46" t="s">
+      <c r="C90" s="46" t="s">
         <v>542</v>
       </c>
-      <c r="C90" s="46" t="s">
+      <c r="D90" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="D90" s="47" t="s">
+      <c r="H90" s="46" t="s">
+        <v>541</v>
+      </c>
+      <c r="I90" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="J90" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="M90" s="46" t="s">
+        <v>541</v>
+      </c>
+      <c r="N90" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="O90" s="47" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B91" s="46" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="46" t="s">
-        <v>545</v>
-      </c>
       <c r="C91" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D91" s="47"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="46" t="s">
-        <v>548</v>
-      </c>
-      <c r="C92" s="46" t="s">
-        <v>439</v>
-      </c>
-      <c r="D92" s="47" t="s">
-        <v>549</v>
-      </c>
+      <c r="H91" s="46" t="s">
+        <v>555</v>
+      </c>
+      <c r="I91" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" s="47" t="s">
+        <v>556</v>
+      </c>
+      <c r="M91" s="46"/>
+      <c r="N91" s="46"/>
+      <c r="O91" s="47"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B92" s="46"/>
+      <c r="C92" s="46"/>
+      <c r="D92" s="47"/>
+      <c r="H92" s="46"/>
+      <c r="I92" s="46"/>
+      <c r="J92" s="47"/>
+      <c r="M92" s="46"/>
+      <c r="N92" s="46"/>
+      <c r="O92" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revision 17 Ago USA
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Axis\Axis website\axis\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,189 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FIELD VALUES'!$C$60:$E$233</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>aelavalle</author>
+  </authors>
+  <commentList>
+    <comment ref="H99" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Agregar os campos que falten. NO dan en la tabla de herramientas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B104" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Glove Bag</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B105" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Notes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B117" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Glove Bag</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B118" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Notes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B128" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Glove Bag</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B129" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>aelavalle:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="599">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -1713,6 +1890,117 @@
   </si>
   <si>
     <t>TABLE: SHIPPINGS</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Serial #</t>
+  </si>
+  <si>
+    <t>Serial 2 #</t>
+  </si>
+  <si>
+    <t>Additiona 1</t>
+  </si>
+  <si>
+    <t>Additiona 2</t>
+  </si>
+  <si>
+    <t>Status / Condition</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rescue Kits</t>
+  </si>
+  <si>
+    <t>PO / TECH</t>
+  </si>
+  <si>
+    <t>Tool Kits</t>
+  </si>
+  <si>
+    <t>40 Cal Suit</t>
+  </si>
+  <si>
+    <t>Class 0 Gloves</t>
+  </si>
+  <si>
+    <t>Class 0 Face Shield</t>
+  </si>
+  <si>
+    <t>Tic Tracer</t>
+  </si>
+  <si>
+    <t>Torque Wrench</t>
+  </si>
+  <si>
+    <t>Torque Pump</t>
+  </si>
+  <si>
+    <t>Hot Stick</t>
+  </si>
+  <si>
+    <t>LOTO Box</t>
+  </si>
+  <si>
+    <t>Hard Hat</t>
+  </si>
+  <si>
+    <t>Harness</t>
+  </si>
+  <si>
+    <t>Lanyard</t>
+  </si>
+  <si>
+    <t>Lad-Saf</t>
+  </si>
+  <si>
+    <t>Calibration Due / Manufact. Date</t>
+  </si>
+  <si>
+    <t>Assign to Tuck / VIN</t>
+  </si>
+  <si>
+    <t>Commets</t>
+  </si>
+  <si>
+    <t>Only 1 per Tuck</t>
+  </si>
+  <si>
+    <t>JOB</t>
+  </si>
+  <si>
+    <t>Cada PPE es asignado a un solo tecnico</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Asignar a un solo JOB, lo mismo que los Tecnicos</t>
+  </si>
+  <si>
+    <t>ContractId</t>
+  </si>
+  <si>
+    <t>JOB / Warehouse</t>
+  </si>
+  <si>
+    <t>TruckId</t>
+  </si>
+  <si>
+    <t>Truck / Warehouse</t>
+  </si>
+  <si>
+    <t>TABLE: ASSIGNMENT OF TOOLS BY JOB</t>
+  </si>
+  <si>
+    <t>TABLE: ASSIGNMENT OF TOOLS BY TRUCK</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +2010,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1796,8 +2084,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1825,6 +2126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,7 +2333,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2085,6 +2392,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3175,11 +3490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M89" sqref="M89"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,8 +3507,8 @@
     <col min="6" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="44.140625" customWidth="1"/>
     <col min="11" max="12" width="3.7109375" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
@@ -6770,10 +7085,419 @@
       <c r="N92" s="46"/>
       <c r="O92" s="47"/>
     </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B95" s="44" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B96" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B97" s="46" t="s">
+        <v>593</v>
+      </c>
+      <c r="C97" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="D97" s="47"/>
+      <c r="H97" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="H98" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="H99" s="48" t="s">
+        <v>573</v>
+      </c>
+      <c r="I99" s="48" t="s">
+        <v>589</v>
+      </c>
+      <c r="J99" s="48" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="H100" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="H101" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="H102" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="H103" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="H104" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="H105" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B106" s="40" t="s">
+        <v>591</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H107" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B108" s="44" t="s">
+        <v>598</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B109" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B110" s="46" t="s">
+        <v>595</v>
+      </c>
+      <c r="C110" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="D110" s="47"/>
+      <c r="H110" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D114" s="1"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="1"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D116" s="1"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D117" s="1"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="40" t="s">
+        <v>591</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="49"/>
+      <c r="C120" s="49"/>
+      <c r="D120" s="49"/>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="50"/>
+      <c r="C121" s="50"/>
+      <c r="D121" s="51"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="52"/>
+      <c r="C122" s="52"/>
+      <c r="D122" s="52"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="52"/>
+      <c r="C123" s="52"/>
+      <c r="D123" s="52"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="52"/>
+      <c r="C124" s="52"/>
+      <c r="D124" s="52"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="52"/>
+      <c r="C125" s="52"/>
+      <c r="D125" s="52"/>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="52"/>
+      <c r="C126" s="52"/>
+      <c r="D126" s="52"/>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="52"/>
+      <c r="C127" s="52"/>
+      <c r="D127" s="52"/>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="52"/>
+      <c r="C128" s="52"/>
+      <c r="D128" s="52"/>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="52"/>
+      <c r="C129" s="52"/>
+      <c r="D129" s="52"/>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="53"/>
+      <c r="C130" s="52"/>
+      <c r="D130" s="52"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se agrega TruckDetails y Tabla Truckdetails
Se agrega el modulo donde se generan los registros para capturar
información sobre los autos rentados.
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Axis\Axis website\axis\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="607">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -2001,6 +2001,30 @@
   </si>
   <si>
     <t>TABLE: ASSIGNMENT OF TOOLS BY TRUCK</t>
+  </si>
+  <si>
+    <t>TABLE: TruckDetails</t>
+  </si>
+  <si>
+    <t>PlateNumber</t>
+  </si>
+  <si>
+    <t>Numero de placa</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Other 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>Este campo ayuda a determinar si ya fueron colocados la cantidad de autos a rentar</t>
   </si>
 </sst>
 </file>
@@ -3488,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A94" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F79" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6885,7 +6909,7 @@
       </c>
       <c r="D80" s="32"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B81" s="31" t="s">
         <v>475</v>
       </c>
@@ -6894,7 +6918,7 @@
       </c>
       <c r="D81" s="31"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B85" s="44" t="s">
         <v>538</v>
       </c>
@@ -6902,10 +6926,13 @@
         <v>549</v>
       </c>
       <c r="M85" t="s">
+        <v>599</v>
+      </c>
+      <c r="R85" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B86" s="45" t="s">
         <v>0</v>
       </c>
@@ -6933,8 +6960,17 @@
       <c r="O86" s="45" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R86" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="S86" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="T86" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B87" s="46" t="s">
         <v>547</v>
       </c>
@@ -6954,16 +6990,23 @@
         <v>548</v>
       </c>
       <c r="M87" s="46" t="s">
-        <v>547</v>
+        <v>595</v>
       </c>
       <c r="N87" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="O87" s="47" t="s">
+      <c r="O87" s="47"/>
+      <c r="R87" s="46" t="s">
+        <v>547</v>
+      </c>
+      <c r="S87" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="T87" s="47" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="88" spans="2:15" ht="68.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:20" ht="57" x14ac:dyDescent="0.25">
       <c r="B88" s="46" t="s">
         <v>539</v>
       </c>
@@ -6983,16 +7026,25 @@
         <v>551</v>
       </c>
       <c r="M88" s="46" t="s">
+        <v>600</v>
+      </c>
+      <c r="N88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="47" t="s">
+        <v>601</v>
+      </c>
+      <c r="R88" s="46" t="s">
         <v>557</v>
       </c>
-      <c r="N88" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="O88" s="47" t="s">
+      <c r="S88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="T88" s="47" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="89" spans="2:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="46" t="s">
         <v>546</v>
       </c>
@@ -7012,14 +7064,21 @@
         <v>553</v>
       </c>
       <c r="M89" s="46" t="s">
+        <v>603</v>
+      </c>
+      <c r="N89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O89" s="47"/>
+      <c r="R89" s="46" t="s">
         <v>559</v>
       </c>
-      <c r="N89" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="O89" s="47"/>
-    </row>
-    <row r="90" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="S89" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="T89" s="47"/>
+    </row>
+    <row r="90" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B90" s="46" t="s">
         <v>541</v>
       </c>
@@ -7039,16 +7098,23 @@
         <v>554</v>
       </c>
       <c r="M90" s="46" t="s">
+        <v>563</v>
+      </c>
+      <c r="N90" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O90" s="47"/>
+      <c r="R90" s="46" t="s">
         <v>541</v>
       </c>
-      <c r="N90" s="46" t="s">
+      <c r="S90" s="46" t="s">
         <v>542</v>
       </c>
-      <c r="O90" s="47" t="s">
+      <c r="T90" s="47" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B91" s="46" t="s">
         <v>544</v>
       </c>
@@ -7065,27 +7131,47 @@
       <c r="J91" s="47" t="s">
         <v>556</v>
       </c>
-      <c r="M91" s="46"/>
-      <c r="N91" s="46"/>
+      <c r="M91" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="N91" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="O91" s="47"/>
-    </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R91" s="46"/>
+      <c r="S91" s="46"/>
+      <c r="T91" s="47"/>
+    </row>
+    <row r="92" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B92" s="46"/>
       <c r="C92" s="46"/>
       <c r="D92" s="47"/>
-      <c r="H92" s="46"/>
-      <c r="I92" s="46"/>
-      <c r="J92" s="47"/>
-      <c r="M92" s="46"/>
-      <c r="N92" s="46"/>
+      <c r="H92" s="46" t="s">
+        <v>605</v>
+      </c>
+      <c r="I92" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="J92" s="47" t="s">
+        <v>606</v>
+      </c>
+      <c r="M92" s="46" t="s">
+        <v>604</v>
+      </c>
+      <c r="N92" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="O92" s="47"/>
-    </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R92" s="46"/>
+      <c r="S92" s="46"/>
+      <c r="T92" s="47"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B95" s="44" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B96" s="45" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de tabla de Truck Details
</commit_message>
<xml_diff>
--- a/Documentacion/DBASE MODEL V2 PPT.xlsx
+++ b/Documentacion/DBASE MODEL V2 PPT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\axis\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Axis\Axis website\axis\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="643">
   <si>
     <t>FIELD NAME</t>
   </si>
@@ -2006,25 +2006,133 @@
     <t>TABLE: TruckDetails</t>
   </si>
   <si>
-    <t>PlateNumber</t>
-  </si>
-  <si>
     <t>Numero de placa</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Other 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Status </t>
   </si>
   <si>
     <t>Este campo ayuda a determinar si ya fueron colocados la cantidad de autos a rentar</t>
+  </si>
+  <si>
+    <t>Licence Plate</t>
+  </si>
+  <si>
+    <t>MakeModel</t>
+  </si>
+  <si>
+    <t>Site Location</t>
+  </si>
+  <si>
+    <t>Last 6 of VIN</t>
+  </si>
+  <si>
+    <t>Date Rent</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Gas/Diesel</t>
+  </si>
+  <si>
+    <t>Gas Card</t>
+  </si>
+  <si>
+    <t>Yes/NO</t>
+  </si>
+  <si>
+    <t>Insurance Documentacion</t>
+  </si>
+  <si>
+    <t>Item Interior 1</t>
+  </si>
+  <si>
+    <t>Item Interior 2</t>
+  </si>
+  <si>
+    <t>Item Interior 3</t>
+  </si>
+  <si>
+    <t>Item Interior 4</t>
+  </si>
+  <si>
+    <t>Item Interior 5</t>
+  </si>
+  <si>
+    <t>Engine Comparment 1</t>
+  </si>
+  <si>
+    <t>Engine Comparment 2</t>
+  </si>
+  <si>
+    <t>Engine Comparment 3</t>
+  </si>
+  <si>
+    <t>Engine Comparment 4</t>
+  </si>
+  <si>
+    <t>Item exterior 1</t>
+  </si>
+  <si>
+    <t>Item exterior 2</t>
+  </si>
+  <si>
+    <t>Item exterior 3</t>
+  </si>
+  <si>
+    <t>Item exterior 4</t>
+  </si>
+  <si>
+    <t>Item exterior 5</t>
+  </si>
+  <si>
+    <t>Item exterior 6</t>
+  </si>
+  <si>
+    <t>Item exterior 7</t>
+  </si>
+  <si>
+    <t>Item exterior 8</t>
+  </si>
+  <si>
+    <t>Item exterior 9</t>
+  </si>
+  <si>
+    <t>Item exterior 10</t>
+  </si>
+  <si>
+    <t>Item exterior 11</t>
+  </si>
+  <si>
+    <t>Item exterior 12</t>
+  </si>
+  <si>
+    <t>Item exterior 13</t>
+  </si>
+  <si>
+    <t>Item exterior 14</t>
+  </si>
+  <si>
+    <t>Item exterior 15</t>
+  </si>
+  <si>
+    <t>Item exterior 16</t>
+  </si>
+  <si>
+    <t>Aditional Comments</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Dia de renta</t>
+  </si>
+  <si>
+    <t>Ultimos dígitos del VIN</t>
+  </si>
+  <si>
+    <t>Model / Marca</t>
   </si>
 </sst>
 </file>
@@ -3512,8 +3620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F79" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N100" sqref="N100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7026,13 +7134,13 @@
         <v>551</v>
       </c>
       <c r="M88" s="46" t="s">
+        <v>603</v>
+      </c>
+      <c r="N88" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="47" t="s">
         <v>600</v>
-      </c>
-      <c r="N88" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="O88" s="47" t="s">
-        <v>601</v>
       </c>
       <c r="R88" s="46" t="s">
         <v>557</v>
@@ -7064,12 +7172,14 @@
         <v>553</v>
       </c>
       <c r="M89" s="46" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="N89" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="O89" s="47"/>
+      <c r="O89" s="47" t="s">
+        <v>642</v>
+      </c>
       <c r="R89" s="46" t="s">
         <v>559</v>
       </c>
@@ -7098,7 +7208,7 @@
         <v>554</v>
       </c>
       <c r="M90" s="46" t="s">
-        <v>563</v>
+        <v>605</v>
       </c>
       <c r="N90" s="46" t="s">
         <v>18</v>
@@ -7132,12 +7242,14 @@
         <v>556</v>
       </c>
       <c r="M91" s="46" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="N91" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="O91" s="47"/>
+      <c r="O91" s="47" t="s">
+        <v>641</v>
+      </c>
       <c r="R91" s="46"/>
       <c r="S91" s="46"/>
       <c r="T91" s="47"/>
@@ -7147,29 +7259,62 @@
       <c r="C92" s="46"/>
       <c r="D92" s="47"/>
       <c r="H92" s="46" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="I92" s="46" t="s">
         <v>18</v>
       </c>
       <c r="J92" s="47" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="M92" s="46" t="s">
-        <v>604</v>
-      </c>
-      <c r="N92" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="O92" s="47"/>
+        <v>607</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O92" s="47" t="s">
+        <v>640</v>
+      </c>
       <c r="R92" s="46"/>
       <c r="S92" s="46"/>
       <c r="T92" s="47"/>
     </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M93" s="46" t="s">
+        <v>608</v>
+      </c>
+      <c r="N93" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M94" s="46" t="s">
+        <v>609</v>
+      </c>
+      <c r="N94" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
     <row r="95" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B95" s="44" t="s">
         <v>597</v>
       </c>
+      <c r="M95" s="46" t="s">
+        <v>610</v>
+      </c>
+      <c r="N95" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="96" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B96" s="45" t="s">
@@ -7190,8 +7335,17 @@
       <c r="J96" s="1" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M96" s="46" t="s">
+        <v>612</v>
+      </c>
+      <c r="N96" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="46" t="s">
         <v>593</v>
       </c>
@@ -7208,8 +7362,17 @@
       <c r="J97" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M97" s="46" t="s">
+        <v>613</v>
+      </c>
+      <c r="N97" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>562</v>
       </c>
@@ -7226,8 +7389,17 @@
       <c r="J98" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M98" s="46" t="s">
+        <v>614</v>
+      </c>
+      <c r="N98" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>563</v>
       </c>
@@ -7244,8 +7416,17 @@
       <c r="J99" s="48" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M99" s="46" t="s">
+        <v>615</v>
+      </c>
+      <c r="N99" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>564</v>
       </c>
@@ -7262,8 +7443,17 @@
       <c r="J100" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M100" s="46" t="s">
+        <v>616</v>
+      </c>
+      <c r="N100" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>565</v>
       </c>
@@ -7280,8 +7470,17 @@
       <c r="J101" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M101" s="46" t="s">
+        <v>617</v>
+      </c>
+      <c r="N101" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>568</v>
       </c>
@@ -7298,8 +7497,17 @@
       <c r="J102" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M102" s="46" t="s">
+        <v>618</v>
+      </c>
+      <c r="N102" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>585</v>
       </c>
@@ -7316,8 +7524,17 @@
       <c r="J103" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M103" s="46" t="s">
+        <v>619</v>
+      </c>
+      <c r="N103" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>566</v>
       </c>
@@ -7334,8 +7551,17 @@
       <c r="J104" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M104" s="46" t="s">
+        <v>620</v>
+      </c>
+      <c r="N104" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>567</v>
       </c>
@@ -7352,8 +7578,17 @@
       <c r="J105" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M105" s="46" t="s">
+        <v>621</v>
+      </c>
+      <c r="N105" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="40" t="s">
         <v>591</v>
       </c>
@@ -7372,8 +7607,17 @@
       <c r="J106" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M106" s="46" t="s">
+        <v>622</v>
+      </c>
+      <c r="N106" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" s="40" t="s">
         <v>569</v>
       </c>
@@ -7390,8 +7634,17 @@
       <c r="J107" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M107" s="46" t="s">
+        <v>623</v>
+      </c>
+      <c r="N107" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H108" s="1" t="s">
         <v>582</v>
       </c>
@@ -7401,8 +7654,17 @@
       <c r="J108" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M108" s="46" t="s">
+        <v>624</v>
+      </c>
+      <c r="N108" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109" s="44" t="s">
         <v>598</v>
       </c>
@@ -7415,8 +7677,17 @@
       <c r="J109" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M109" s="46" t="s">
+        <v>625</v>
+      </c>
+      <c r="N109" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="s">
         <v>0</v>
       </c>
@@ -7435,8 +7706,17 @@
       <c r="J110" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M110" s="46" t="s">
+        <v>626</v>
+      </c>
+      <c r="N110" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111" s="46" t="s">
         <v>595</v>
       </c>
@@ -7444,8 +7724,17 @@
         <v>439</v>
       </c>
       <c r="D111" s="47"/>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M111" s="46" t="s">
+        <v>627</v>
+      </c>
+      <c r="N111" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>562</v>
       </c>
@@ -7453,8 +7742,17 @@
         <v>18</v>
       </c>
       <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M112" s="46" t="s">
+        <v>628</v>
+      </c>
+      <c r="N112" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>563</v>
       </c>
@@ -7462,8 +7760,17 @@
         <v>18</v>
       </c>
       <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M113" s="46" t="s">
+        <v>629</v>
+      </c>
+      <c r="N113" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>564</v>
       </c>
@@ -7471,8 +7778,17 @@
         <v>18</v>
       </c>
       <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M114" s="46" t="s">
+        <v>630</v>
+      </c>
+      <c r="N114" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
         <v>565</v>
       </c>
@@ -7480,8 +7796,17 @@
         <v>18</v>
       </c>
       <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M115" s="46" t="s">
+        <v>631</v>
+      </c>
+      <c r="N115" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
         <v>568</v>
       </c>
@@ -7489,8 +7814,17 @@
         <v>18</v>
       </c>
       <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M116" s="46" t="s">
+        <v>632</v>
+      </c>
+      <c r="N116" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>585</v>
       </c>
@@ -7498,8 +7832,17 @@
         <v>105</v>
       </c>
       <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M117" s="46" t="s">
+        <v>633</v>
+      </c>
+      <c r="N117" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
         <v>566</v>
       </c>
@@ -7507,8 +7850,17 @@
         <v>18</v>
       </c>
       <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M118" s="46" t="s">
+        <v>634</v>
+      </c>
+      <c r="N118" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
         <v>567</v>
       </c>
@@ -7516,8 +7868,17 @@
         <v>18</v>
       </c>
       <c r="D119" s="1"/>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M119" s="46" t="s">
+        <v>635</v>
+      </c>
+      <c r="N119" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B120" s="40" t="s">
         <v>591</v>
       </c>
@@ -7527,8 +7888,17 @@
       <c r="D120" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M120" s="46" t="s">
+        <v>636</v>
+      </c>
+      <c r="N120" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121" s="40" t="s">
         <v>569</v>
       </c>
@@ -7536,38 +7906,56 @@
         <v>18</v>
       </c>
       <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M121" s="46" t="s">
+        <v>637</v>
+      </c>
+      <c r="N121" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122" s="49"/>
       <c r="C122" s="49"/>
       <c r="D122" s="49"/>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M122" s="46" t="s">
+        <v>638</v>
+      </c>
+      <c r="N122" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123" s="49"/>
       <c r="C123" s="49"/>
       <c r="D123" s="49"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124" s="49"/>
       <c r="C124" s="49"/>
       <c r="D124" s="49"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125" s="49"/>
       <c r="C125" s="49"/>
       <c r="D125" s="49"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B126" s="49"/>
       <c r="C126" s="49"/>
       <c r="D126" s="49"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B127" s="49"/>
       <c r="C127" s="49"/>
       <c r="D127" s="49"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B128" s="49"/>
       <c r="C128" s="49"/>
       <c r="D128" s="49"/>

</xml_diff>